<commit_message>
Updates to roll 1.7.0.0 release
Added Armor +1 token
Key Map updated
Help file updated
Apprentice Modes added
</commit_message>
<xml_diff>
--- a/Template/OCTGN - Key Map.xlsx
+++ b/Template/OCTGN - Key Map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="222">
   <si>
     <t>Voltaric</t>
   </si>
@@ -513,27 +513,18 @@
     <t>Alt R</t>
   </si>
   <si>
-    <t>Add  Corrode Token</t>
-  </si>
-  <si>
     <t>Add Growth Marker</t>
   </si>
   <si>
     <t>Enter</t>
   </si>
   <si>
-    <t>Add Bleed Token</t>
-  </si>
-  <si>
     <t>Add Stuck Marker</t>
   </si>
   <si>
     <t>Remove Stuck Marker</t>
   </si>
   <si>
-    <t>Remove Bleed Token</t>
-  </si>
-  <si>
     <t>Remove Growth Marker</t>
   </si>
   <si>
@@ -615,10 +606,91 @@
     <t>Reveal your Enchantment?</t>
   </si>
   <si>
-    <t>Show Rose Compass</t>
-  </si>
-  <si>
     <t>2x3 Apprentice Arena</t>
+  </si>
+  <si>
+    <t>3x3 Apprentice Arena</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>Remove Rot Marker</t>
+  </si>
+  <si>
+    <t>Add Slam Marker</t>
+  </si>
+  <si>
+    <t>Remove Slam Marker</t>
+  </si>
+  <si>
+    <t>Add Stun Marker</t>
+  </si>
+  <si>
+    <t>Remove Stun Marker</t>
+  </si>
+  <si>
+    <t>Add Weak Marker</t>
+  </si>
+  <si>
+    <t>Remove Weak Marker</t>
+  </si>
+  <si>
+    <t>Add Burn Marker</t>
+  </si>
+  <si>
+    <t>Remove Burn Marker</t>
+  </si>
+  <si>
+    <t>Add Bleed Marker</t>
+  </si>
+  <si>
+    <t>Remove Bleed Marker</t>
+  </si>
+  <si>
+    <t>Add  Corrode Marker</t>
+  </si>
+  <si>
+    <t>Remove Corrode Marker</t>
+  </si>
+  <si>
+    <t>Add Cripple Marker</t>
+  </si>
+  <si>
+    <t>Remove Cripple Marker</t>
+  </si>
+  <si>
+    <t>Add Daze Marker</t>
+  </si>
+  <si>
+    <t>Remove Daze Marker</t>
+  </si>
+  <si>
+    <t>Add Disable Marker</t>
+  </si>
+  <si>
+    <t>Remove Disable Marker</t>
+  </si>
+  <si>
+    <t>Add Other Marker/Token</t>
+  </si>
+  <si>
+    <t>Remove All Markers/Tokens</t>
+  </si>
+  <si>
+    <t>Show Compass Rose</t>
+  </si>
+  <si>
+    <t>Add Mana Counter</t>
+  </si>
+  <si>
+    <t>Remove Mana Counter</t>
+  </si>
+  <si>
+    <t>Add Armor +1 Marker</t>
+  </si>
+  <si>
+    <t>Remove Armor +1 Marker</t>
   </si>
 </sst>
 </file>
@@ -679,7 +751,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -725,6 +797,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -802,7 +880,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -849,19 +927,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1177,10 +1266,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="24"/>
-      <c r="B1" s="24"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="A1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2362,10 +2451,10 @@
       <c r="L30" t="s">
         <v>112</v>
       </c>
-      <c r="M30" s="22" t="s">
+      <c r="M30" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="N30" s="22"/>
+      <c r="N30" s="27"/>
     </row>
     <row r="31" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
@@ -2386,10 +2475,10 @@
       <c r="L31" t="s">
         <v>98</v>
       </c>
-      <c r="M31" s="22" t="s">
+      <c r="M31" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="N31" s="22"/>
+      <c r="N31" s="27"/>
     </row>
     <row r="32" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
@@ -2401,10 +2490,10 @@
       <c r="L32" t="s">
         <v>119</v>
       </c>
-      <c r="M32" s="22" t="s">
+      <c r="M32" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="N32" s="22"/>
+      <c r="N32" s="27"/>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
@@ -2419,19 +2508,19 @@
       <c r="L33" t="s">
         <v>127</v>
       </c>
-      <c r="M33" s="22" t="s">
+      <c r="M33" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="N33" s="22"/>
+      <c r="N33" s="27"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="L34" t="s">
         <v>118</v>
       </c>
-      <c r="M34" s="22" t="s">
+      <c r="M34" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="N34" s="22"/>
+      <c r="N34" s="27"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
@@ -2443,19 +2532,19 @@
       <c r="L35" t="s">
         <v>123</v>
       </c>
-      <c r="M35" s="23" t="s">
+      <c r="M35" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="N35" s="23"/>
+      <c r="N35" s="28"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="L36" t="s">
         <v>124</v>
       </c>
-      <c r="M36" s="23" t="s">
+      <c r="M36" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="N36" s="23"/>
+      <c r="N36" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2479,27 +2568,28 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.77734375" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.88671875" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.77734375" customWidth="1"/>
     <col min="9" max="9" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.88671875" style="23" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2.77734375" customWidth="1"/>
-    <col min="14" max="14" width="2.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.77734375" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2.77734375" customWidth="1"/>
-    <col min="18" max="18" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.77734375" style="23" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="2.77734375" customWidth="1"/>
     <col min="21" max="21" width="10.5546875" bestFit="1" customWidth="1"/>
@@ -2508,1464 +2598,1476 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="25"/>
-      <c r="B1" s="25"/>
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
       <c r="C1" s="19"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>93</v>
       </c>
       <c r="D2" s="20"/>
-      <c r="E2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>64</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>147</v>
+        <v>216</v>
       </c>
       <c r="H2" s="20"/>
-      <c r="I2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="I2" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>64</v>
       </c>
+      <c r="K2" s="21" t="s">
+        <v>220</v>
+      </c>
       <c r="L2" s="20"/>
-      <c r="M2" t="s">
-        <v>134</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="M2" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="N2" s="25" t="s">
         <v>64</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>221</v>
       </c>
       <c r="P2" s="20"/>
       <c r="Q2" t="s">
         <v>151</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="23" t="s">
         <v>64</v>
       </c>
       <c r="T2" s="20"/>
-      <c r="U2" t="s">
+      <c r="U2" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="V2" s="28" t="s">
+      <c r="V2" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="W2" s="28"/>
+      <c r="W2" s="32"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="25" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>121</v>
+        <v>203</v>
       </c>
       <c r="D3" s="20"/>
-      <c r="E3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>65</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>145</v>
+        <v>204</v>
       </c>
       <c r="H3" s="20"/>
-      <c r="I3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="I3" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="25" t="s">
         <v>65</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>165</v>
+        <v>205</v>
       </c>
       <c r="L3" s="20"/>
-      <c r="M3" t="s">
-        <v>134</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="M3" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="N3" s="25" t="s">
         <v>65</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>168</v>
+        <v>206</v>
       </c>
       <c r="P3" s="20"/>
       <c r="Q3" t="s">
         <v>151</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="23" t="s">
         <v>65</v>
       </c>
       <c r="T3" s="20"/>
-      <c r="U3" t="s">
+      <c r="U3" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="V3" s="28" t="s">
+      <c r="V3" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="W3" s="28"/>
+      <c r="W3" s="32"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>66</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>162</v>
+        <v>207</v>
       </c>
       <c r="D4" s="20"/>
-      <c r="E4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>66</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>152</v>
+        <v>208</v>
       </c>
       <c r="H4" s="20"/>
-      <c r="I4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="I4" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="25" t="s">
         <v>66</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>104</v>
+        <v>209</v>
       </c>
       <c r="L4" s="20"/>
-      <c r="M4" t="s">
-        <v>134</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="M4" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="N4" s="25" t="s">
         <v>66</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>150</v>
+        <v>210</v>
       </c>
       <c r="P4" s="20"/>
       <c r="Q4" t="s">
         <v>151</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="23" t="s">
         <v>66</v>
       </c>
       <c r="T4" s="20"/>
-      <c r="U4" t="s">
+      <c r="U4" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>100</v>
+        <v>211</v>
       </c>
       <c r="D5" s="20"/>
-      <c r="E5" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="25" t="s">
         <v>67</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>146</v>
+        <v>212</v>
       </c>
       <c r="H5" s="20"/>
-      <c r="I5" t="s">
-        <v>90</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="I5" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5" s="25" t="s">
         <v>67</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>157</v>
+        <v>213</v>
       </c>
       <c r="L5" s="20"/>
-      <c r="M5" t="s">
-        <v>134</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="M5" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="N5" s="25" t="s">
         <v>67</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>155</v>
+        <v>214</v>
       </c>
       <c r="P5" s="20"/>
-      <c r="Q5" t="s">
-        <v>151</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="Q5" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="R5" s="25" t="s">
         <v>67</v>
       </c>
       <c r="S5" s="21" t="s">
         <v>97</v>
       </c>
       <c r="T5" s="20"/>
-      <c r="U5" t="s">
+      <c r="U5" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="V5" s="28" t="s">
+      <c r="V5" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="W5" s="28"/>
+      <c r="W5" s="32"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>68</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>140</v>
       </c>
       <c r="D6" s="20"/>
-      <c r="E6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6" s="26" t="s">
         <v>68</v>
       </c>
       <c r="H6" s="20"/>
-      <c r="I6" t="s">
-        <v>90</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="I6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" s="26" t="s">
         <v>68</v>
       </c>
       <c r="L6" s="20"/>
-      <c r="M6" t="s">
-        <v>134</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="M6" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N6" s="26" t="s">
         <v>68</v>
       </c>
       <c r="P6" s="20"/>
       <c r="Q6" t="s">
         <v>151</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="23" t="s">
         <v>68</v>
       </c>
       <c r="T6" s="20"/>
-      <c r="U6" t="s">
+      <c r="U6" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="V6" s="28" t="s">
+      <c r="V6" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="28"/>
+      <c r="W6" s="32"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>69</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>114</v>
       </c>
       <c r="D7" s="20"/>
-      <c r="E7" t="s">
-        <v>132</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="26" t="s">
         <v>69</v>
       </c>
       <c r="H7" s="20"/>
-      <c r="I7" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="I7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="26" t="s">
         <v>69</v>
       </c>
       <c r="L7" s="20"/>
-      <c r="M7" t="s">
-        <v>134</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="M7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N7" s="26" t="s">
         <v>69</v>
       </c>
       <c r="P7" s="20"/>
       <c r="Q7" t="s">
         <v>151</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="23" t="s">
         <v>69</v>
       </c>
       <c r="T7" s="20"/>
-      <c r="U7" t="s">
-        <v>123</v>
-      </c>
-      <c r="V7" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="W7" s="23"/>
+      <c r="U7" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="V7" s="21" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>70</v>
       </c>
       <c r="C8" s="21" t="s">
         <v>111</v>
       </c>
       <c r="D8" s="20"/>
-      <c r="E8" t="s">
-        <v>132</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="E8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="26" t="s">
         <v>70</v>
       </c>
       <c r="H8" s="20"/>
-      <c r="I8" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="I8" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="25" t="s">
         <v>70</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L8" s="20"/>
-      <c r="M8" t="s">
-        <v>134</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="M8" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="N8" s="25" t="s">
         <v>70</v>
       </c>
       <c r="O8" s="21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="P8" s="20"/>
       <c r="Q8" t="s">
         <v>151</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="23" t="s">
         <v>70</v>
       </c>
       <c r="T8" s="20"/>
-      <c r="U8" t="s">
-        <v>124</v>
-      </c>
-      <c r="V8" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="W8" s="23"/>
+      <c r="U8" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="V8" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="W8" s="28"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>71</v>
       </c>
       <c r="D9" s="20"/>
-      <c r="E9" t="s">
-        <v>132</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="E9" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" s="26" t="s">
         <v>71</v>
       </c>
       <c r="H9" s="20"/>
-      <c r="I9" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="I9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="26" t="s">
         <v>71</v>
       </c>
       <c r="L9" s="20"/>
-      <c r="M9" t="s">
-        <v>134</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="M9" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N9" s="26" t="s">
         <v>71</v>
       </c>
       <c r="P9" s="20"/>
       <c r="Q9" t="s">
         <v>151</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="23" t="s">
         <v>71</v>
       </c>
       <c r="T9" s="20"/>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
+      <c r="U9" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="V9" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="W9" s="22"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="A10" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>72</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>106</v>
       </c>
       <c r="D10" s="20"/>
-      <c r="E10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E10" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="26" t="s">
         <v>72</v>
       </c>
       <c r="H10" s="20"/>
-      <c r="I10" t="s">
-        <v>90</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="I10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="26" t="s">
         <v>72</v>
       </c>
       <c r="L10" s="20"/>
-      <c r="M10" t="s">
-        <v>134</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="M10" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N10" s="26" t="s">
         <v>72</v>
       </c>
       <c r="P10" s="20"/>
       <c r="Q10" t="s">
         <v>151</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="23" t="s">
         <v>72</v>
       </c>
       <c r="T10" s="20"/>
-      <c r="V10" s="26"/>
-      <c r="W10" s="26"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="A11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="20"/>
-      <c r="E11" t="s">
-        <v>132</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="E11" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="26" t="s">
         <v>73</v>
       </c>
       <c r="H11" s="20"/>
-      <c r="I11" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="I11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="26" t="s">
         <v>73</v>
       </c>
       <c r="L11" s="20"/>
-      <c r="M11" t="s">
-        <v>134</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="M11" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N11" s="26" t="s">
         <v>73</v>
       </c>
       <c r="P11" s="20"/>
       <c r="Q11" t="s">
         <v>151</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="23" t="s">
         <v>73</v>
       </c>
       <c r="T11" s="20"/>
-      <c r="V11" s="26"/>
-      <c r="W11" s="26"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="A12" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="25" t="s">
         <v>74</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D12" s="20"/>
-      <c r="E12" t="s">
-        <v>132</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" s="25" t="s">
         <v>74</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H12" s="20"/>
-      <c r="I12" t="s">
-        <v>90</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="I12" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="26" t="s">
         <v>74</v>
       </c>
       <c r="L12" s="20"/>
-      <c r="M12" t="s">
-        <v>134</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="M12" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N12" s="26" t="s">
         <v>74</v>
       </c>
       <c r="P12" s="20"/>
       <c r="Q12" t="s">
         <v>151</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12" s="23" t="s">
         <v>74</v>
       </c>
       <c r="T12" s="20"/>
-      <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="33"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="25" t="s">
         <v>75</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>92</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="E13" t="s">
-        <v>132</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="E13" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F13" s="26" t="s">
         <v>75</v>
       </c>
       <c r="H13" s="20"/>
-      <c r="I13" t="s">
-        <v>90</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="I13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13" s="26" t="s">
         <v>75</v>
       </c>
       <c r="L13" s="20"/>
-      <c r="M13" t="s">
-        <v>134</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="M13" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N13" s="26" t="s">
         <v>75</v>
       </c>
       <c r="P13" s="20"/>
       <c r="Q13" t="s">
         <v>151</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="23" t="s">
         <v>75</v>
       </c>
       <c r="T13" s="20"/>
-      <c r="V13" s="26"/>
-      <c r="W13" s="26"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="33"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="A14" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="25" t="s">
         <v>76</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>99</v>
+        <v>218</v>
       </c>
       <c r="D14" s="20"/>
-      <c r="E14" t="s">
-        <v>132</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="E14" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" s="25" t="s">
         <v>76</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>144</v>
+        <v>219</v>
       </c>
       <c r="H14" s="20"/>
-      <c r="I14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="I14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="26" t="s">
         <v>76</v>
       </c>
       <c r="L14" s="20"/>
-      <c r="M14" t="s">
-        <v>134</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="M14" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N14" s="26" t="s">
         <v>76</v>
       </c>
       <c r="P14" s="20"/>
       <c r="Q14" t="s">
         <v>151</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14" s="23" t="s">
         <v>76</v>
       </c>
       <c r="T14" s="20"/>
-      <c r="V14" s="26"/>
-      <c r="W14" s="26"/>
+      <c r="V14" s="33"/>
+      <c r="W14" s="33"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="A15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="26" t="s">
         <v>77</v>
       </c>
       <c r="D15" s="20"/>
-      <c r="E15" t="s">
-        <v>132</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="E15" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" s="26" t="s">
         <v>77</v>
       </c>
       <c r="H15" s="20"/>
-      <c r="I15" t="s">
-        <v>90</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="I15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J15" s="26" t="s">
         <v>77</v>
       </c>
       <c r="L15" s="20"/>
-      <c r="M15" t="s">
-        <v>134</v>
-      </c>
-      <c r="N15" t="s">
+      <c r="M15" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N15" s="26" t="s">
         <v>77</v>
       </c>
       <c r="P15" s="20"/>
       <c r="Q15" t="s">
         <v>151</v>
       </c>
-      <c r="R15" t="s">
+      <c r="R15" s="23" t="s">
         <v>77</v>
       </c>
       <c r="T15" s="20"/>
-      <c r="V15" s="26"/>
-      <c r="W15" s="26"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="33"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="A16" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>78</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>105</v>
+        <v>215</v>
       </c>
       <c r="D16" s="20"/>
-      <c r="E16" t="s">
-        <v>132</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="E16" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F16" s="26" t="s">
         <v>78</v>
       </c>
       <c r="H16" s="20"/>
-      <c r="I16" t="s">
-        <v>90</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="I16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" s="26" t="s">
         <v>78</v>
       </c>
       <c r="L16" s="20"/>
-      <c r="M16" t="s">
-        <v>134</v>
-      </c>
-      <c r="N16" t="s">
+      <c r="M16" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N16" s="26" t="s">
         <v>78</v>
       </c>
       <c r="P16" s="20"/>
       <c r="Q16" t="s">
         <v>151</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16" s="23" t="s">
         <v>78</v>
       </c>
       <c r="T16" s="20"/>
-      <c r="V16" s="26"/>
-      <c r="W16" s="26"/>
+      <c r="V16" s="33"/>
+      <c r="W16" s="33"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="A17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="26" t="s">
         <v>79</v>
       </c>
       <c r="D17" s="20"/>
-      <c r="E17" t="s">
-        <v>132</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="E17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" s="26" t="s">
         <v>79</v>
       </c>
       <c r="H17" s="20"/>
-      <c r="I17" t="s">
-        <v>90</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="I17" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" s="25" t="s">
         <v>79</v>
       </c>
       <c r="K17" s="21" t="s">
         <v>139</v>
       </c>
       <c r="L17" s="20"/>
-      <c r="M17" t="s">
-        <v>134</v>
-      </c>
-      <c r="N17" t="s">
+      <c r="M17" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N17" s="26" t="s">
         <v>79</v>
       </c>
       <c r="P17" s="20"/>
       <c r="Q17" t="s">
         <v>151</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="23" t="s">
         <v>79</v>
       </c>
       <c r="T17" s="20"/>
-      <c r="V17" s="26"/>
-      <c r="W17" s="26"/>
+      <c r="V17" s="33"/>
+      <c r="W17" s="33"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="A18" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>80</v>
       </c>
       <c r="C18" s="21" t="s">
         <v>110</v>
       </c>
       <c r="D18" s="20"/>
-      <c r="E18" t="s">
-        <v>132</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E18" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" s="26" t="s">
         <v>80</v>
       </c>
       <c r="H18" s="20"/>
-      <c r="I18" t="s">
-        <v>90</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="I18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" s="26" t="s">
         <v>80</v>
       </c>
       <c r="L18" s="20"/>
-      <c r="M18" t="s">
-        <v>134</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="M18" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N18" s="26" t="s">
         <v>80</v>
       </c>
       <c r="P18" s="20"/>
       <c r="Q18" t="s">
         <v>151</v>
       </c>
-      <c r="R18" t="s">
+      <c r="R18" s="23" t="s">
         <v>80</v>
       </c>
       <c r="T18" s="20"/>
-      <c r="V18" s="26"/>
-      <c r="W18" s="26"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="A19" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="25" t="s">
         <v>81</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>94</v>
       </c>
       <c r="D19" s="20"/>
-      <c r="E19" t="s">
-        <v>132</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="E19" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="25" t="s">
         <v>81</v>
       </c>
       <c r="G19" s="21" t="s">
         <v>135</v>
       </c>
       <c r="H19" s="20"/>
-      <c r="I19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="I19" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" s="25" t="s">
         <v>81</v>
       </c>
       <c r="K19" s="21" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L19" s="20"/>
-      <c r="M19" t="s">
-        <v>134</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="M19" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="N19" s="25" t="s">
         <v>81</v>
       </c>
       <c r="O19" s="21" t="s">
-        <v>156</v>
+        <v>196</v>
       </c>
       <c r="P19" s="20"/>
       <c r="Q19" t="s">
         <v>151</v>
       </c>
-      <c r="R19" t="s">
+      <c r="R19" s="23" t="s">
         <v>81</v>
       </c>
       <c r="T19" s="20"/>
-      <c r="V19" s="26"/>
-      <c r="W19" s="26"/>
+      <c r="V19" s="33"/>
+      <c r="W19" s="33"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="A20" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="25" t="s">
         <v>82</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>102</v>
+        <v>197</v>
       </c>
       <c r="D20" s="20"/>
-      <c r="E20" t="s">
-        <v>132</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="E20" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" s="25" t="s">
         <v>82</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
       <c r="H20" s="20"/>
-      <c r="I20" t="s">
-        <v>90</v>
-      </c>
-      <c r="J20" t="s">
+      <c r="I20" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J20" s="25" t="s">
         <v>82</v>
       </c>
       <c r="K20" s="21" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
       <c r="L20" s="20"/>
-      <c r="M20" t="s">
-        <v>134</v>
-      </c>
-      <c r="N20" t="s">
+      <c r="M20" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="N20" s="25" t="s">
         <v>82</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>148</v>
+        <v>200</v>
       </c>
       <c r="P20" s="20"/>
       <c r="Q20" t="s">
         <v>151</v>
       </c>
-      <c r="R20" t="s">
+      <c r="R20" s="23" t="s">
         <v>82</v>
       </c>
       <c r="T20" s="20"/>
-      <c r="V20" s="26"/>
-      <c r="W20" s="26"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="33"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="25" t="s">
         <v>83</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>91</v>
       </c>
       <c r="D21" s="20"/>
-      <c r="E21" t="s">
-        <v>132</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E21" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" s="26" t="s">
         <v>83</v>
       </c>
       <c r="H21" s="20"/>
-      <c r="I21" t="s">
-        <v>90</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="I21" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="25" t="s">
         <v>83</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="L21" s="20"/>
-      <c r="M21" t="s">
-        <v>134</v>
-      </c>
-      <c r="N21" t="s">
+      <c r="M21" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="N21" s="25" t="s">
         <v>83</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="P21" s="20"/>
       <c r="Q21" t="s">
         <v>151</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R21" s="23" t="s">
         <v>83</v>
       </c>
       <c r="T21" s="20"/>
-      <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
+      <c r="V21" s="33"/>
+      <c r="W21" s="33"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="A22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="26" t="s">
         <v>84</v>
       </c>
       <c r="D22" s="20"/>
-      <c r="E22" t="s">
-        <v>132</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E22" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="26" t="s">
         <v>84</v>
       </c>
       <c r="H22" s="20"/>
-      <c r="I22" t="s">
-        <v>90</v>
-      </c>
-      <c r="J22" t="s">
+      <c r="I22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="26" t="s">
         <v>84</v>
       </c>
       <c r="L22" s="20"/>
-      <c r="M22" t="s">
-        <v>134</v>
-      </c>
-      <c r="N22" t="s">
+      <c r="M22" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="N22" s="26" t="s">
         <v>84</v>
       </c>
       <c r="P22" s="20"/>
       <c r="Q22" t="s">
         <v>151</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R22" s="23" t="s">
         <v>84</v>
       </c>
       <c r="T22" s="20"/>
-      <c r="V22" s="26"/>
-      <c r="W22" s="26"/>
+      <c r="V22" s="33"/>
+      <c r="W22" s="33"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="A23" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>85</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>95</v>
       </c>
       <c r="D23" s="20"/>
-      <c r="E23" t="s">
-        <v>132</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="E23" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23" s="26" t="s">
         <v>85</v>
       </c>
       <c r="H23" s="20"/>
-      <c r="I23" t="s">
-        <v>90</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="I23" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" s="25" t="s">
         <v>85</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L23" s="20"/>
-      <c r="M23" t="s">
-        <v>134</v>
-      </c>
-      <c r="N23" t="s">
+      <c r="M23" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="N23" s="25" t="s">
         <v>85</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="P23" s="20"/>
       <c r="Q23" t="s">
         <v>151</v>
       </c>
-      <c r="R23" t="s">
+      <c r="R23" s="23" t="s">
         <v>85</v>
       </c>
       <c r="T23" s="20"/>
-      <c r="V23" s="26"/>
-      <c r="W23" s="26"/>
+      <c r="V23" s="33"/>
+      <c r="W23" s="33"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="A24" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="25" t="s">
         <v>86</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="D24" s="20"/>
-      <c r="E24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="E24" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="25" t="s">
         <v>86</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>149</v>
+        <v>202</v>
       </c>
       <c r="H24" s="20"/>
-      <c r="I24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="I24" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" s="26" t="s">
         <v>86</v>
       </c>
       <c r="L24" s="20"/>
       <c r="M24" t="s">
         <v>134</v>
       </c>
-      <c r="N24" t="s">
+      <c r="N24" s="23" t="s">
         <v>86</v>
       </c>
       <c r="P24" s="20"/>
       <c r="Q24" t="s">
         <v>151</v>
       </c>
-      <c r="R24" t="s">
+      <c r="R24" s="23" t="s">
         <v>86</v>
       </c>
       <c r="T24" s="20"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="33"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="A25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="26" t="s">
         <v>87</v>
       </c>
       <c r="D25" s="20"/>
-      <c r="E25" t="s">
-        <v>132</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E25" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F25" s="26" t="s">
         <v>87</v>
       </c>
       <c r="H25" s="20"/>
-      <c r="I25" t="s">
-        <v>90</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="I25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J25" s="26" t="s">
         <v>87</v>
       </c>
       <c r="L25" s="20"/>
       <c r="M25" t="s">
         <v>134</v>
       </c>
-      <c r="N25" t="s">
+      <c r="N25" s="23" t="s">
         <v>87</v>
       </c>
       <c r="P25" s="20"/>
       <c r="Q25" t="s">
         <v>151</v>
       </c>
-      <c r="R25" t="s">
+      <c r="R25" s="23" t="s">
         <v>87</v>
       </c>
       <c r="T25" s="20"/>
-      <c r="V25" s="26"/>
-      <c r="W25" s="26"/>
+      <c r="V25" s="33"/>
+      <c r="W25" s="33"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="A26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="26" t="s">
         <v>88</v>
       </c>
       <c r="D26" s="20"/>
-      <c r="E26" t="s">
-        <v>132</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F26" s="26" t="s">
         <v>88</v>
       </c>
       <c r="H26" s="20"/>
-      <c r="I26" t="s">
-        <v>90</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="I26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J26" s="26" t="s">
         <v>88</v>
       </c>
       <c r="L26" s="20"/>
       <c r="M26" t="s">
         <v>134</v>
       </c>
-      <c r="N26" t="s">
+      <c r="N26" s="23" t="s">
         <v>88</v>
       </c>
       <c r="P26" s="20"/>
       <c r="Q26" t="s">
         <v>151</v>
       </c>
-      <c r="R26" t="s">
+      <c r="R26" s="23" t="s">
         <v>88</v>
       </c>
       <c r="T26" s="20"/>
-      <c r="V26" s="26"/>
-      <c r="W26" s="26"/>
+      <c r="V26" s="33"/>
+      <c r="W26" s="33"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="A27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="26" t="s">
         <v>89</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D27" s="20"/>
-      <c r="E27" t="s">
-        <v>132</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="E27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="26" t="s">
         <v>89</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H27" s="20"/>
-      <c r="I27" t="s">
-        <v>90</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="I27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J27" s="26" t="s">
         <v>89</v>
       </c>
       <c r="L27" s="20"/>
       <c r="M27" t="s">
         <v>134</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N27" s="23" t="s">
         <v>89</v>
       </c>
       <c r="P27" s="20"/>
       <c r="Q27" t="s">
         <v>151</v>
       </c>
-      <c r="R27" t="s">
+      <c r="R27" s="23" t="s">
         <v>89</v>
       </c>
       <c r="T27" s="20"/>
-      <c r="V27" s="26"/>
-      <c r="W27" s="26"/>
+      <c r="V27" s="33"/>
+      <c r="W27" s="33"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="A28" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="25" t="s">
         <v>115</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>116</v>
       </c>
       <c r="D28" s="20"/>
-      <c r="E28" t="s">
-        <v>132</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="E28" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F28" s="25" t="s">
         <v>137</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>159</v>
       </c>
       <c r="H28" s="20"/>
-      <c r="I28" t="s">
-        <v>90</v>
-      </c>
-      <c r="J28" t="s">
-        <v>118</v>
+      <c r="I28" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J28" s="25" t="s">
+        <v>112</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="L28" s="20"/>
       <c r="P28" s="20"/>
       <c r="T28" s="20"/>
-      <c r="V28" s="26"/>
-      <c r="W28" s="26"/>
+      <c r="V28" s="33"/>
+      <c r="W28" s="33"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="25" t="s">
         <v>130</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>131</v>
       </c>
       <c r="D29" s="20"/>
-      <c r="E29" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
+      <c r="E29" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
       <c r="H29" s="20"/>
-      <c r="I29" t="s">
-        <v>90</v>
-      </c>
-      <c r="J29" t="s">
-        <v>112</v>
+      <c r="I29" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="25" t="s">
+        <v>98</v>
       </c>
       <c r="K29" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="L29" s="20"/>
       <c r="P29" s="20"/>
       <c r="T29" s="20"/>
-      <c r="V29" s="26"/>
-      <c r="W29" s="26"/>
+      <c r="V29" s="33"/>
+      <c r="W29" s="33"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="25" t="s">
         <v>136</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>138</v>
       </c>
       <c r="D30" s="20"/>
-      <c r="E30" t="s">
-        <v>132</v>
-      </c>
-      <c r="F30">
+      <c r="E30" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F30" s="25">
         <v>1</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H30" s="20"/>
-      <c r="I30" t="s">
-        <v>90</v>
-      </c>
-      <c r="J30" t="s">
-        <v>98</v>
+      <c r="I30" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="25" t="s">
+        <v>119</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="L30" s="20"/>
       <c r="P30" s="20"/>
       <c r="T30" s="20"/>
-      <c r="V30" s="26"/>
-      <c r="W30" s="26"/>
+      <c r="V30" s="33"/>
+      <c r="W30" s="33"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="A31" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="25" t="s">
         <v>141</v>
       </c>
       <c r="C31" s="21" t="s">
         <v>143</v>
       </c>
       <c r="D31" s="20"/>
-      <c r="E31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F31">
+      <c r="E31" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="25">
         <v>2</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H31" s="20"/>
-      <c r="I31" t="s">
-        <v>90</v>
-      </c>
-      <c r="J31" t="s">
-        <v>119</v>
+      <c r="I31" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="25" t="s">
+        <v>127</v>
       </c>
       <c r="K31" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L31" s="20"/>
       <c r="P31" s="20"/>
       <c r="T31" s="20"/>
-      <c r="V31" s="26"/>
-      <c r="W31" s="26"/>
+      <c r="V31" s="33"/>
+      <c r="W31" s="33"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" t="s">
-        <v>164</v>
+      <c r="A32" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>163</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>116</v>
       </c>
       <c r="D32" s="20"/>
-      <c r="E32" t="s">
-        <v>132</v>
-      </c>
-      <c r="F32">
+      <c r="E32" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F32" s="25">
         <v>3</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H32" s="20"/>
-      <c r="I32" t="s">
-        <v>90</v>
-      </c>
-      <c r="J32" t="s">
-        <v>127</v>
+      <c r="I32" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32" s="25" t="s">
+        <v>174</v>
       </c>
       <c r="K32" s="21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="L32" s="20"/>
       <c r="P32" s="20"/>
       <c r="T32" s="20"/>
-      <c r="V32" s="26"/>
-      <c r="W32" s="26"/>
+      <c r="V32" s="33"/>
+      <c r="W32" s="33"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="26"/>
       <c r="D33" s="20"/>
-      <c r="E33" t="s">
-        <v>132</v>
-      </c>
-      <c r="F33">
+      <c r="E33" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F33" s="25">
         <v>4</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H33" s="20"/>
-      <c r="I33" t="s">
-        <v>90</v>
-      </c>
-      <c r="J33" t="s">
-        <v>177</v>
+      <c r="I33" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J33" s="25" t="s">
+        <v>195</v>
       </c>
       <c r="K33" s="21" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="L33" s="20"/>
       <c r="P33" s="20"/>
       <c r="T33" s="20"/>
-      <c r="V33" s="26"/>
-      <c r="W33" s="26"/>
+      <c r="V33" s="33"/>
+      <c r="W33" s="33"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="A34" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="25" t="s">
         <v>112</v>
       </c>
       <c r="C34" s="21" t="s">
         <v>120</v>
       </c>
       <c r="D34" s="20"/>
-      <c r="E34" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34">
+      <c r="E34" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="25">
         <v>5</v>
       </c>
       <c r="G34" s="21" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H34" s="20"/>
-      <c r="I34" t="s">
-        <v>90</v>
-      </c>
-      <c r="J34" t="s">
+      <c r="I34" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J34" s="25" t="s">
         <v>137</v>
       </c>
       <c r="K34" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L34" s="20"/>
       <c r="P34" s="20"/>
       <c r="T34" s="20"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="A35" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="25" t="s">
         <v>98</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="D35" s="20"/>
-      <c r="E35" t="s">
-        <v>132</v>
-      </c>
-      <c r="F35">
+      <c r="E35" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="25">
         <v>6</v>
       </c>
       <c r="G35" s="21" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H35" s="20"/>
-      <c r="I35" t="s">
-        <v>90</v>
-      </c>
-      <c r="J35" t="s">
-        <v>178</v>
+      <c r="I35" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J35" s="25" t="s">
+        <v>175</v>
       </c>
       <c r="K35" s="21" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L35" s="20"/>
       <c r="P35" s="20"/>
@@ -3973,24 +4075,24 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D36" s="20"/>
-      <c r="E36" t="s">
-        <v>132</v>
-      </c>
-      <c r="F36">
+      <c r="E36" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="25">
         <v>7</v>
       </c>
       <c r="G36" s="21" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H36" s="20"/>
-      <c r="I36" t="s">
-        <v>90</v>
-      </c>
-      <c r="J36" t="s">
-        <v>179</v>
+      <c r="I36" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J36" s="25" t="s">
+        <v>176</v>
       </c>
       <c r="K36" s="21" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="L36" s="20"/>
       <c r="P36" s="20"/>
@@ -3998,32 +4100,48 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D37" s="20"/>
-      <c r="E37" t="s">
-        <v>132</v>
-      </c>
-      <c r="F37">
+      <c r="E37" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F37" s="25">
         <v>8</v>
       </c>
       <c r="G37" s="21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H37" s="20"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="26"/>
       <c r="L37" s="20"/>
       <c r="P37" s="20"/>
       <c r="T37" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="32">
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="V22:W22"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="V6:W6"/>
-    <mergeCell ref="V7:W7"/>
     <mergeCell ref="V8:W8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="V1:W1"/>
-    <mergeCell ref="V9:W9"/>
     <mergeCell ref="V10:W10"/>
     <mergeCell ref="V11:W11"/>
     <mergeCell ref="V12:W12"/>
@@ -4032,22 +4150,6 @@
     <mergeCell ref="V15:W15"/>
     <mergeCell ref="V16:W16"/>
     <mergeCell ref="V17:W17"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#117- Added Melee +1 Marker
- all FvW markers resized to 200x200
- lint and nits cleaned up in the FvW set.xml
</commit_message>
<xml_diff>
--- a/Template/OCTGN - Key Map.xlsx
+++ b/Template/OCTGN - Key Map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="224">
   <si>
     <t>Voltaric</t>
   </si>
@@ -691,6 +691,12 @@
   </si>
   <si>
     <t>Remove Armor +1 Marker</t>
+  </si>
+  <si>
+    <t>Add Melee +1 Marker</t>
+  </si>
+  <si>
+    <t>Remove Melee +1 Marker</t>
   </si>
 </sst>
 </file>
@@ -944,13 +950,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2567,8 +2573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2587,7 +2593,7 @@
     <col min="12" max="12" width="2.77734375" customWidth="1"/>
     <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2.77734375" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2.77734375" customWidth="1"/>
     <col min="18" max="18" width="2.77734375" style="23" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
@@ -2601,8 +2607,8 @@
       <c r="A1" s="30"/>
       <c r="B1" s="30"/>
       <c r="C1" s="19"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
@@ -2655,10 +2661,10 @@
       <c r="U2" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="V2" s="32" t="s">
+      <c r="V2" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="W2" s="32"/>
+      <c r="W2" s="33"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -2711,10 +2717,10 @@
       <c r="U3" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="V3" s="32" t="s">
+      <c r="V3" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="W3" s="32"/>
+      <c r="W3" s="33"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
@@ -2822,10 +2828,10 @@
       <c r="U5" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="V5" s="32" t="s">
+      <c r="V5" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="W5" s="32"/>
+      <c r="W5" s="33"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
@@ -2869,10 +2875,10 @@
       <c r="U6" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="V6" s="32" t="s">
+      <c r="V6" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="32"/>
+      <c r="W6" s="33"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
@@ -3056,8 +3062,8 @@
         <v>72</v>
       </c>
       <c r="T10" s="20"/>
-      <c r="V10" s="33"/>
-      <c r="W10" s="33"/>
+      <c r="V10" s="31"/>
+      <c r="W10" s="31"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -3095,8 +3101,8 @@
         <v>73</v>
       </c>
       <c r="T11" s="20"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="33"/>
+      <c r="V11" s="31"/>
+      <c r="W11" s="31"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
@@ -3140,8 +3146,8 @@
         <v>74</v>
       </c>
       <c r="T12" s="20"/>
-      <c r="V12" s="33"/>
-      <c r="W12" s="33"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -3182,8 +3188,8 @@
         <v>75</v>
       </c>
       <c r="T13" s="20"/>
-      <c r="V13" s="33"/>
-      <c r="W13" s="33"/>
+      <c r="V13" s="31"/>
+      <c r="W13" s="31"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -3206,18 +3212,24 @@
         <v>219</v>
       </c>
       <c r="H14" s="20"/>
-      <c r="I14" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J14" s="26" t="s">
+      <c r="I14" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="25" t="s">
         <v>76</v>
       </c>
+      <c r="K14" s="21" t="s">
+        <v>222</v>
+      </c>
       <c r="L14" s="20"/>
-      <c r="M14" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="N14" s="26" t="s">
+      <c r="M14" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="N14" s="25" t="s">
         <v>76</v>
+      </c>
+      <c r="O14" s="21" t="s">
+        <v>223</v>
       </c>
       <c r="P14" s="20"/>
       <c r="Q14" t="s">
@@ -3227,8 +3239,8 @@
         <v>76</v>
       </c>
       <c r="T14" s="20"/>
-      <c r="V14" s="33"/>
-      <c r="W14" s="33"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -3266,8 +3278,8 @@
         <v>77</v>
       </c>
       <c r="T15" s="20"/>
-      <c r="V15" s="33"/>
-      <c r="W15" s="33"/>
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
@@ -3308,8 +3320,8 @@
         <v>78</v>
       </c>
       <c r="T16" s="20"/>
-      <c r="V16" s="33"/>
-      <c r="W16" s="33"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="31"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -3350,8 +3362,8 @@
         <v>79</v>
       </c>
       <c r="T17" s="20"/>
-      <c r="V17" s="33"/>
-      <c r="W17" s="33"/>
+      <c r="V17" s="31"/>
+      <c r="W17" s="31"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
@@ -3392,8 +3404,8 @@
         <v>80</v>
       </c>
       <c r="T18" s="20"/>
-      <c r="V18" s="33"/>
-      <c r="W18" s="33"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
@@ -3443,8 +3455,8 @@
         <v>81</v>
       </c>
       <c r="T19" s="20"/>
-      <c r="V19" s="33"/>
-      <c r="W19" s="33"/>
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
@@ -3494,8 +3506,8 @@
         <v>82</v>
       </c>
       <c r="T20" s="20"/>
-      <c r="V20" s="33"/>
-      <c r="W20" s="33"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
@@ -3542,8 +3554,8 @@
         <v>83</v>
       </c>
       <c r="T21" s="20"/>
-      <c r="V21" s="33"/>
-      <c r="W21" s="33"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="31"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
@@ -3581,8 +3593,8 @@
         <v>84</v>
       </c>
       <c r="T22" s="20"/>
-      <c r="V22" s="33"/>
-      <c r="W22" s="33"/>
+      <c r="V22" s="31"/>
+      <c r="W22" s="31"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
@@ -3629,8 +3641,8 @@
         <v>85</v>
       </c>
       <c r="T23" s="20"/>
-      <c r="V23" s="33"/>
-      <c r="W23" s="33"/>
+      <c r="V23" s="31"/>
+      <c r="W23" s="31"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
@@ -3674,8 +3686,8 @@
         <v>86</v>
       </c>
       <c r="T24" s="20"/>
-      <c r="V24" s="33"/>
-      <c r="W24" s="33"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -3713,8 +3725,8 @@
         <v>87</v>
       </c>
       <c r="T25" s="20"/>
-      <c r="V25" s="33"/>
-      <c r="W25" s="33"/>
+      <c r="V25" s="31"/>
+      <c r="W25" s="31"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -3752,24 +3764,24 @@
         <v>88</v>
       </c>
       <c r="T26" s="20"/>
-      <c r="V26" s="33"/>
-      <c r="W26" s="33"/>
+      <c r="V26" s="31"/>
+      <c r="W26" s="31"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="25" t="s">
         <v>89</v>
       </c>
       <c r="C27" s="21" t="s">
         <v>172</v>
       </c>
       <c r="D27" s="20"/>
-      <c r="E27" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F27" s="26" t="s">
+      <c r="E27" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="25" t="s">
         <v>89</v>
       </c>
       <c r="G27" s="21" t="s">
@@ -3797,8 +3809,8 @@
         <v>89</v>
       </c>
       <c r="T27" s="20"/>
-      <c r="V27" s="33"/>
-      <c r="W27" s="33"/>
+      <c r="V27" s="31"/>
+      <c r="W27" s="31"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
@@ -3833,8 +3845,8 @@
       <c r="L28" s="20"/>
       <c r="P28" s="20"/>
       <c r="T28" s="20"/>
-      <c r="V28" s="33"/>
-      <c r="W28" s="33"/>
+      <c r="V28" s="31"/>
+      <c r="W28" s="31"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
@@ -3847,11 +3859,11 @@
         <v>131</v>
       </c>
       <c r="D29" s="20"/>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
       <c r="H29" s="20"/>
       <c r="I29" s="24" t="s">
         <v>90</v>
@@ -3865,8 +3877,8 @@
       <c r="L29" s="20"/>
       <c r="P29" s="20"/>
       <c r="T29" s="20"/>
-      <c r="V29" s="33"/>
-      <c r="W29" s="33"/>
+      <c r="V29" s="31"/>
+      <c r="W29" s="31"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
@@ -3901,8 +3913,8 @@
       <c r="L30" s="20"/>
       <c r="P30" s="20"/>
       <c r="T30" s="20"/>
-      <c r="V30" s="33"/>
-      <c r="W30" s="33"/>
+      <c r="V30" s="31"/>
+      <c r="W30" s="31"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
@@ -3937,8 +3949,8 @@
       <c r="L31" s="20"/>
       <c r="P31" s="20"/>
       <c r="T31" s="20"/>
-      <c r="V31" s="33"/>
-      <c r="W31" s="33"/>
+      <c r="V31" s="31"/>
+      <c r="W31" s="31"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
@@ -3973,8 +3985,8 @@
       <c r="L32" s="20"/>
       <c r="P32" s="20"/>
       <c r="T32" s="20"/>
-      <c r="V32" s="33"/>
-      <c r="W32" s="33"/>
+      <c r="V32" s="31"/>
+      <c r="W32" s="31"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
@@ -4002,8 +4014,8 @@
       <c r="L33" s="20"/>
       <c r="P33" s="20"/>
       <c r="T33" s="20"/>
-      <c r="V33" s="33"/>
-      <c r="W33" s="33"/>
+      <c r="V33" s="31"/>
+      <c r="W33" s="31"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
@@ -4118,22 +4130,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="V22:W22"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="V6:W6"/>
     <mergeCell ref="V8:W8"/>
@@ -4150,6 +4146,22 @@
     <mergeCell ref="V15:W15"/>
     <mergeCell ref="V16:W16"/>
     <mergeCell ref="V17:W17"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V29:W29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#148 - Added Keyboard Shortcuts for Ranged +1 Markers
#171 - Added Keyboard Shortcut for accessing the Codex - Ctrl+H
</commit_message>
<xml_diff>
--- a/Template/OCTGN - Key Map.xlsx
+++ b/Template/OCTGN - Key Map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Github\Mage-Wars\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Mage-Wars\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="227">
   <si>
     <t>Voltaric</t>
   </si>
@@ -697,6 +697,15 @@
   </si>
   <si>
     <t>Remove Melee +1 Marker</t>
+  </si>
+  <si>
+    <t>Search Codex</t>
+  </si>
+  <si>
+    <t>Add Ranged +1 Marker</t>
+  </si>
+  <si>
+    <t>Remove Ranged +1 Marker</t>
   </si>
 </sst>
 </file>
@@ -950,13 +959,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2574,7 +2583,7 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2607,8 +2616,8 @@
       <c r="A1" s="30"/>
       <c r="B1" s="30"/>
       <c r="C1" s="19"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
@@ -2661,10 +2670,10 @@
       <c r="U2" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="V2" s="33" t="s">
+      <c r="V2" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="W2" s="33"/>
+      <c r="W2" s="32"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -2717,10 +2726,10 @@
       <c r="U3" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="V3" s="33" t="s">
+      <c r="V3" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="W3" s="33"/>
+      <c r="W3" s="32"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
@@ -2828,10 +2837,10 @@
       <c r="U5" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="V5" s="33" t="s">
+      <c r="V5" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="W5" s="33"/>
+      <c r="W5" s="32"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
@@ -2875,10 +2884,10 @@
       <c r="U6" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="V6" s="33" t="s">
+      <c r="V6" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="33"/>
+      <c r="W6" s="32"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
@@ -2980,11 +2989,14 @@
       <c r="W8" s="28"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="26" t="s">
+      <c r="A9" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>71</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>224</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="2" t="s">
@@ -3062,8 +3074,8 @@
         <v>72</v>
       </c>
       <c r="T10" s="20"/>
-      <c r="V10" s="31"/>
-      <c r="W10" s="31"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -3101,8 +3113,8 @@
         <v>73</v>
       </c>
       <c r="T11" s="20"/>
-      <c r="V11" s="31"/>
-      <c r="W11" s="31"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
@@ -3146,8 +3158,8 @@
         <v>74</v>
       </c>
       <c r="T12" s="20"/>
-      <c r="V12" s="31"/>
-      <c r="W12" s="31"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="33"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -3188,8 +3200,8 @@
         <v>75</v>
       </c>
       <c r="T13" s="20"/>
-      <c r="V13" s="31"/>
-      <c r="W13" s="31"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="33"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -3239,22 +3251,28 @@
         <v>76</v>
       </c>
       <c r="T14" s="20"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
+      <c r="V14" s="33"/>
+      <c r="W14" s="33"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="26" t="s">
+      <c r="A15" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="25" t="s">
         <v>77</v>
       </c>
+      <c r="C15" s="21" t="s">
+        <v>225</v>
+      </c>
       <c r="D15" s="20"/>
-      <c r="E15" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F15" s="26" t="s">
+      <c r="E15" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" s="25" t="s">
         <v>77</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>226</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="2" t="s">
@@ -3278,8 +3296,8 @@
         <v>77</v>
       </c>
       <c r="T15" s="20"/>
-      <c r="V15" s="31"/>
-      <c r="W15" s="31"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="33"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
@@ -3320,8 +3338,8 @@
         <v>78</v>
       </c>
       <c r="T16" s="20"/>
-      <c r="V16" s="31"/>
-      <c r="W16" s="31"/>
+      <c r="V16" s="33"/>
+      <c r="W16" s="33"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -3362,8 +3380,8 @@
         <v>79</v>
       </c>
       <c r="T17" s="20"/>
-      <c r="V17" s="31"/>
-      <c r="W17" s="31"/>
+      <c r="V17" s="33"/>
+      <c r="W17" s="33"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
@@ -3404,8 +3422,8 @@
         <v>80</v>
       </c>
       <c r="T18" s="20"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
@@ -3455,8 +3473,8 @@
         <v>81</v>
       </c>
       <c r="T19" s="20"/>
-      <c r="V19" s="31"/>
-      <c r="W19" s="31"/>
+      <c r="V19" s="33"/>
+      <c r="W19" s="33"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
@@ -3506,8 +3524,8 @@
         <v>82</v>
       </c>
       <c r="T20" s="20"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="31"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="33"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
@@ -3554,8 +3572,8 @@
         <v>83</v>
       </c>
       <c r="T21" s="20"/>
-      <c r="V21" s="31"/>
-      <c r="W21" s="31"/>
+      <c r="V21" s="33"/>
+      <c r="W21" s="33"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
@@ -3593,8 +3611,8 @@
         <v>84</v>
       </c>
       <c r="T22" s="20"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
+      <c r="V22" s="33"/>
+      <c r="W22" s="33"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
@@ -3641,8 +3659,8 @@
         <v>85</v>
       </c>
       <c r="T23" s="20"/>
-      <c r="V23" s="31"/>
-      <c r="W23" s="31"/>
+      <c r="V23" s="33"/>
+      <c r="W23" s="33"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
@@ -3686,8 +3704,8 @@
         <v>86</v>
       </c>
       <c r="T24" s="20"/>
-      <c r="V24" s="31"/>
-      <c r="W24" s="31"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="33"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
@@ -3725,8 +3743,8 @@
         <v>87</v>
       </c>
       <c r="T25" s="20"/>
-      <c r="V25" s="31"/>
-      <c r="W25" s="31"/>
+      <c r="V25" s="33"/>
+      <c r="W25" s="33"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -3764,8 +3782,8 @@
         <v>88</v>
       </c>
       <c r="T26" s="20"/>
-      <c r="V26" s="31"/>
-      <c r="W26" s="31"/>
+      <c r="V26" s="33"/>
+      <c r="W26" s="33"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
@@ -3809,8 +3827,8 @@
         <v>89</v>
       </c>
       <c r="T27" s="20"/>
-      <c r="V27" s="31"/>
-      <c r="W27" s="31"/>
+      <c r="V27" s="33"/>
+      <c r="W27" s="33"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
@@ -3845,8 +3863,8 @@
       <c r="L28" s="20"/>
       <c r="P28" s="20"/>
       <c r="T28" s="20"/>
-      <c r="V28" s="31"/>
-      <c r="W28" s="31"/>
+      <c r="V28" s="33"/>
+      <c r="W28" s="33"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
@@ -3859,11 +3877,11 @@
         <v>131</v>
       </c>
       <c r="D29" s="20"/>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
       <c r="H29" s="20"/>
       <c r="I29" s="24" t="s">
         <v>90</v>
@@ -3877,8 +3895,8 @@
       <c r="L29" s="20"/>
       <c r="P29" s="20"/>
       <c r="T29" s="20"/>
-      <c r="V29" s="31"/>
-      <c r="W29" s="31"/>
+      <c r="V29" s="33"/>
+      <c r="W29" s="33"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
@@ -3913,8 +3931,8 @@
       <c r="L30" s="20"/>
       <c r="P30" s="20"/>
       <c r="T30" s="20"/>
-      <c r="V30" s="31"/>
-      <c r="W30" s="31"/>
+      <c r="V30" s="33"/>
+      <c r="W30" s="33"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
@@ -3949,8 +3967,8 @@
       <c r="L31" s="20"/>
       <c r="P31" s="20"/>
       <c r="T31" s="20"/>
-      <c r="V31" s="31"/>
-      <c r="W31" s="31"/>
+      <c r="V31" s="33"/>
+      <c r="W31" s="33"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
@@ -3985,8 +4003,8 @@
       <c r="L32" s="20"/>
       <c r="P32" s="20"/>
       <c r="T32" s="20"/>
-      <c r="V32" s="31"/>
-      <c r="W32" s="31"/>
+      <c r="V32" s="33"/>
+      <c r="W32" s="33"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
@@ -4014,8 +4032,8 @@
       <c r="L33" s="20"/>
       <c r="P33" s="20"/>
       <c r="T33" s="20"/>
-      <c r="V33" s="31"/>
-      <c r="W33" s="31"/>
+      <c r="V33" s="33"/>
+      <c r="W33" s="33"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
@@ -4130,6 +4148,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="V22:W22"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="V6:W6"/>
     <mergeCell ref="V8:W8"/>
@@ -4146,22 +4180,6 @@
     <mergeCell ref="V15:W15"/>
     <mergeCell ref="V16:W16"/>
     <mergeCell ref="V17:W17"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#144 - fixed Sleep shortcuts
Also moved Ranged +1 shortcuts to the ALT to align with the Melee and
Armor +1 shortcuts.

Updated the Key Map Spreadsheet with new key combos
</commit_message>
<xml_diff>
--- a/Template/OCTGN - Key Map.xlsx
+++ b/Template/OCTGN - Key Map.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Github\Mage-Wars\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Mage-Wars\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10848" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10845" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="232">
   <si>
     <t>Voltaric</t>
   </si>
@@ -706,6 +706,21 @@
   </si>
   <si>
     <t>Add Greater Orb Guardian</t>
+  </si>
+  <si>
+    <t>Add Sleep Marker</t>
+  </si>
+  <si>
+    <t>Remove Sleep Marker</t>
+  </si>
+  <si>
+    <t>Add Ranged +1 Marker</t>
+  </si>
+  <si>
+    <t>Remove Ranged +1 Marker</t>
+  </si>
+  <si>
+    <t>Get Rulings/Clarifications for Card</t>
   </si>
 </sst>
 </file>
@@ -895,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -953,19 +968,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1257,37 +1275,37 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="2.77734375" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" customWidth="1"/>
-    <col min="7" max="7" width="2.77734375" customWidth="1"/>
-    <col min="8" max="8" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.77734375" customWidth="1"/>
-    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.77734375" customWidth="1"/>
-    <col min="14" max="14" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.77734375" customWidth="1"/>
-    <col min="17" max="17" width="3.77734375" customWidth="1"/>
-    <col min="18" max="18" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="2.77734375" customWidth="1"/>
-    <col min="21" max="21" width="3.77734375" customWidth="1"/>
-    <col min="22" max="22" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" customWidth="1"/>
+    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.7109375" customWidth="1"/>
+    <col min="17" max="17" width="3.7109375" customWidth="1"/>
+    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.7109375" customWidth="1"/>
+    <col min="21" max="21" width="3.7109375" customWidth="1"/>
+    <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+    <row r="1" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1331,7 +1349,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1378,7 +1396,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -1428,7 +1446,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
@@ -1478,7 +1496,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
@@ -1519,7 +1537,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
@@ -1560,7 +1578,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1601,7 +1619,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1639,7 +1657,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>18</v>
       </c>
@@ -1680,7 +1698,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>20</v>
       </c>
@@ -1718,7 +1736,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
@@ -1756,7 +1774,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>24</v>
       </c>
@@ -1800,7 +1818,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>26</v>
       </c>
@@ -1844,7 +1862,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
@@ -1882,7 +1900,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>30</v>
       </c>
@@ -1923,7 +1941,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>32</v>
       </c>
@@ -1970,7 +1988,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
@@ -2011,7 +2029,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
@@ -2058,7 +2076,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>38</v>
       </c>
@@ -2108,7 +2126,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>39</v>
       </c>
@@ -2155,7 +2173,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>41</v>
       </c>
@@ -2193,7 +2211,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>43</v>
       </c>
@@ -2234,7 +2252,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>45</v>
       </c>
@@ -2278,7 +2296,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>47</v>
       </c>
@@ -2319,7 +2337,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>49</v>
       </c>
@@ -2357,7 +2375,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>51</v>
       </c>
@@ -2395,7 +2413,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
         <v>53</v>
       </c>
@@ -2430,7 +2448,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>0</v>
       </c>
@@ -2447,7 +2465,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>55</v>
       </c>
@@ -2466,12 +2484,12 @@
       <c r="L30" t="s">
         <v>112</v>
       </c>
-      <c r="M30" s="27" t="s">
+      <c r="M30" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="N30" s="27"/>
-    </row>
-    <row r="31" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N30" s="28"/>
+    </row>
+    <row r="31" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>57</v>
       </c>
@@ -2490,12 +2508,12 @@
       <c r="L31" t="s">
         <v>98</v>
       </c>
-      <c r="M31" s="27" t="s">
+      <c r="M31" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="N31" s="27"/>
-    </row>
-    <row r="32" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N31" s="28"/>
+    </row>
+    <row r="32" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>59</v>
       </c>
@@ -2505,12 +2523,12 @@
       <c r="L32" t="s">
         <v>119</v>
       </c>
-      <c r="M32" s="27" t="s">
+      <c r="M32" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="N32" s="27"/>
-    </row>
-    <row r="33" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N32" s="28"/>
+    </row>
+    <row r="33" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>61</v>
       </c>
@@ -2523,21 +2541,21 @@
       <c r="L33" t="s">
         <v>127</v>
       </c>
-      <c r="M33" s="27" t="s">
+      <c r="M33" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="N33" s="27"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N33" s="28"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L34" t="s">
         <v>118</v>
       </c>
-      <c r="M34" s="27" t="s">
+      <c r="M34" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="N34" s="27"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N34" s="28"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>116</v>
       </c>
@@ -2547,19 +2565,19 @@
       <c r="L35" t="s">
         <v>123</v>
       </c>
-      <c r="M35" s="28" t="s">
+      <c r="M35" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="N35" s="28"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N35" s="29"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L36" t="s">
         <v>124</v>
       </c>
-      <c r="M36" s="28" t="s">
+      <c r="M36" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="N36" s="28"/>
+      <c r="N36" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2582,44 +2600,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.77734375" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.88671875" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.77734375" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" style="23" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.77734375" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.77734375" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.77734375" customWidth="1"/>
-    <col min="18" max="18" width="2.77734375" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" style="23" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="2.77734375" customWidth="1"/>
-    <col min="21" max="21" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.44140625" customWidth="1"/>
-    <col min="23" max="23" width="1.109375" customWidth="1"/>
+    <col min="20" max="20" width="2.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.42578125" customWidth="1"/>
+    <col min="23" max="23" width="1.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
+    <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="19"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>63</v>
       </c>
@@ -2670,12 +2688,12 @@
       <c r="U2" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="V2" s="32" t="s">
+      <c r="V2" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="W2" s="32"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W2" s="34"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>63</v>
       </c>
@@ -2726,12 +2744,12 @@
       <c r="U3" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="V3" s="32" t="s">
+      <c r="V3" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="W3" s="32"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W3" s="34"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>63</v>
       </c>
@@ -2783,7 +2801,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>63</v>
       </c>
@@ -2837,12 +2855,12 @@
       <c r="U5" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="V5" s="32" t="s">
+      <c r="V5" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="W5" s="32"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W5" s="34"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>63</v>
       </c>
@@ -2884,12 +2902,12 @@
       <c r="U6" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="V6" s="32" t="s">
+      <c r="V6" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="32"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="W6" s="34"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>63</v>
       </c>
@@ -2935,7 +2953,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>63</v>
       </c>
@@ -2983,17 +3001,20 @@
       <c r="U8" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="V8" s="28" t="s">
+      <c r="V8" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="W8" s="28"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="26" t="s">
+      <c r="W8" s="29"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>71</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>231</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="2" t="s">
@@ -3032,7 +3053,7 @@
       </c>
       <c r="W9" s="22"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>63</v>
       </c>
@@ -3071,10 +3092,10 @@
         <v>72</v>
       </c>
       <c r="T10" s="20"/>
-      <c r="V10" s="33"/>
-      <c r="W10" s="33"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>63</v>
       </c>
@@ -3110,10 +3131,10 @@
         <v>73</v>
       </c>
       <c r="T11" s="20"/>
-      <c r="V11" s="33"/>
-      <c r="W11" s="33"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V11" s="32"/>
+      <c r="W11" s="32"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>63</v>
       </c>
@@ -3155,10 +3176,10 @@
         <v>74</v>
       </c>
       <c r="T12" s="20"/>
-      <c r="V12" s="33"/>
-      <c r="W12" s="33"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V12" s="32"/>
+      <c r="W12" s="32"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>63</v>
       </c>
@@ -3197,10 +3218,10 @@
         <v>75</v>
       </c>
       <c r="T13" s="20"/>
-      <c r="V13" s="33"/>
-      <c r="W13" s="33"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V13" s="32"/>
+      <c r="W13" s="32"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>63</v>
       </c>
@@ -3248,36 +3269,42 @@
         <v>76</v>
       </c>
       <c r="T14" s="20"/>
-      <c r="V14" s="33"/>
-      <c r="W14" s="33"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="26" t="s">
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>77</v>
       </c>
       <c r="D15" s="20"/>
-      <c r="E15" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F15" s="26" t="s">
+      <c r="E15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" s="27" t="s">
         <v>77</v>
       </c>
       <c r="H15" s="20"/>
-      <c r="I15" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J15" s="26" t="s">
+      <c r="I15" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J15" s="25" t="s">
         <v>77</v>
       </c>
+      <c r="K15" s="21" t="s">
+        <v>229</v>
+      </c>
       <c r="L15" s="20"/>
-      <c r="M15" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="N15" s="26" t="s">
+      <c r="M15" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="N15" s="25" t="s">
         <v>77</v>
+      </c>
+      <c r="O15" s="21" t="s">
+        <v>230</v>
       </c>
       <c r="P15" s="20"/>
       <c r="Q15" t="s">
@@ -3287,10 +3314,10 @@
         <v>77</v>
       </c>
       <c r="T15" s="20"/>
-      <c r="V15" s="33"/>
-      <c r="W15" s="33"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V15" s="32"/>
+      <c r="W15" s="32"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>63</v>
       </c>
@@ -3329,22 +3356,28 @@
         <v>78</v>
       </c>
       <c r="T16" s="20"/>
-      <c r="V16" s="33"/>
-      <c r="W16" s="33"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="26" t="s">
+      <c r="V16" s="32"/>
+      <c r="W16" s="32"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="25" t="s">
         <v>79</v>
       </c>
+      <c r="C17" s="21" t="s">
+        <v>227</v>
+      </c>
       <c r="D17" s="20"/>
-      <c r="E17" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F17" s="26" t="s">
+      <c r="E17" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" s="25" t="s">
         <v>79</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>228</v>
       </c>
       <c r="H17" s="20"/>
       <c r="I17" s="24" t="s">
@@ -3371,10 +3404,10 @@
         <v>79</v>
       </c>
       <c r="T17" s="20"/>
-      <c r="V17" s="33"/>
-      <c r="W17" s="33"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V17" s="32"/>
+      <c r="W17" s="32"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>63</v>
       </c>
@@ -3413,10 +3446,10 @@
         <v>80</v>
       </c>
       <c r="T18" s="20"/>
-      <c r="V18" s="33"/>
-      <c r="W18" s="33"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V18" s="32"/>
+      <c r="W18" s="32"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>63</v>
       </c>
@@ -3464,10 +3497,10 @@
         <v>81</v>
       </c>
       <c r="T19" s="20"/>
-      <c r="V19" s="33"/>
-      <c r="W19" s="33"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V19" s="32"/>
+      <c r="W19" s="32"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>63</v>
       </c>
@@ -3515,10 +3548,10 @@
         <v>82</v>
       </c>
       <c r="T20" s="20"/>
-      <c r="V20" s="33"/>
-      <c r="W20" s="33"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V20" s="32"/>
+      <c r="W20" s="32"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>63</v>
       </c>
@@ -3563,10 +3596,10 @@
         <v>83</v>
       </c>
       <c r="T21" s="20"/>
-      <c r="V21" s="33"/>
-      <c r="W21" s="33"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V21" s="32"/>
+      <c r="W21" s="32"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
@@ -3602,10 +3635,10 @@
         <v>84</v>
       </c>
       <c r="T22" s="20"/>
-      <c r="V22" s="33"/>
-      <c r="W22" s="33"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V22" s="32"/>
+      <c r="W22" s="32"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>63</v>
       </c>
@@ -3650,10 +3683,10 @@
         <v>85</v>
       </c>
       <c r="T23" s="20"/>
-      <c r="V23" s="33"/>
-      <c r="W23" s="33"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V23" s="32"/>
+      <c r="W23" s="32"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>63</v>
       </c>
@@ -3695,10 +3728,10 @@
         <v>86</v>
       </c>
       <c r="T24" s="20"/>
-      <c r="V24" s="33"/>
-      <c r="W24" s="33"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V24" s="32"/>
+      <c r="W24" s="32"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -3734,10 +3767,10 @@
         <v>87</v>
       </c>
       <c r="T25" s="20"/>
-      <c r="V25" s="33"/>
-      <c r="W25" s="33"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V25" s="32"/>
+      <c r="W25" s="32"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
@@ -3773,10 +3806,10 @@
         <v>88</v>
       </c>
       <c r="T26" s="20"/>
-      <c r="V26" s="33"/>
-      <c r="W26" s="33"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V26" s="32"/>
+      <c r="W26" s="32"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
         <v>63</v>
       </c>
@@ -3818,10 +3851,10 @@
         <v>89</v>
       </c>
       <c r="T27" s="20"/>
-      <c r="V27" s="33"/>
-      <c r="W27" s="33"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V27" s="32"/>
+      <c r="W27" s="32"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>63</v>
       </c>
@@ -3854,10 +3887,10 @@
       <c r="L28" s="20"/>
       <c r="P28" s="20"/>
       <c r="T28" s="20"/>
-      <c r="V28" s="33"/>
-      <c r="W28" s="33"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V28" s="32"/>
+      <c r="W28" s="32"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>129</v>
       </c>
@@ -3868,11 +3901,11 @@
         <v>131</v>
       </c>
       <c r="D29" s="20"/>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
       <c r="H29" s="20"/>
       <c r="I29" s="24" t="s">
         <v>90</v>
@@ -3886,10 +3919,10 @@
       <c r="L29" s="20"/>
       <c r="P29" s="20"/>
       <c r="T29" s="20"/>
-      <c r="V29" s="33"/>
-      <c r="W29" s="33"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V29" s="32"/>
+      <c r="W29" s="32"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
         <v>129</v>
       </c>
@@ -3922,10 +3955,10 @@
       <c r="L30" s="20"/>
       <c r="P30" s="20"/>
       <c r="T30" s="20"/>
-      <c r="V30" s="33"/>
-      <c r="W30" s="33"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V30" s="32"/>
+      <c r="W30" s="32"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>63</v>
       </c>
@@ -3958,10 +3991,10 @@
       <c r="L31" s="20"/>
       <c r="P31" s="20"/>
       <c r="T31" s="20"/>
-      <c r="V31" s="33"/>
-      <c r="W31" s="33"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V31" s="32"/>
+      <c r="W31" s="32"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>63</v>
       </c>
@@ -3994,10 +4027,10 @@
       <c r="L32" s="20"/>
       <c r="P32" s="20"/>
       <c r="T32" s="20"/>
-      <c r="V32" s="33"/>
-      <c r="W32" s="33"/>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V32" s="32"/>
+      <c r="W32" s="32"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="26"/>
       <c r="D33" s="20"/>
@@ -4023,10 +4056,10 @@
       <c r="L33" s="20"/>
       <c r="P33" s="20"/>
       <c r="T33" s="20"/>
-      <c r="V33" s="33"/>
-      <c r="W33" s="33"/>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V33" s="32"/>
+      <c r="W33" s="32"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>63</v>
       </c>
@@ -4060,7 +4093,7 @@
       <c r="P34" s="20"/>
       <c r="T34" s="20"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>63</v>
       </c>
@@ -4094,7 +4127,7 @@
       <c r="P35" s="20"/>
       <c r="T35" s="20"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>63</v>
       </c>
@@ -4128,7 +4161,7 @@
       <c r="P36" s="20"/>
       <c r="T36" s="20"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>63</v>
       </c>
@@ -4155,7 +4188,7 @@
       <c r="P37" s="20"/>
       <c r="T37" s="20"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>63</v>
       </c>
@@ -4173,22 +4206,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="V22:W22"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="V6:W6"/>
     <mergeCell ref="V8:W8"/>
@@ -4205,6 +4222,22 @@
     <mergeCell ref="V15:W15"/>
     <mergeCell ref="V16:W16"/>
     <mergeCell ref="V17:W17"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V29:W29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#144 - fixed the other Sleep Shortcut
Updated keyboard map spreadsheet with the above change
</commit_message>
<xml_diff>
--- a/Template/OCTGN - Key Map.xlsx
+++ b/Template/OCTGN - Key Map.xlsx
@@ -910,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -957,7 +957,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -973,17 +972,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1299,10 +1300,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="A1" s="32"/>
+      <c r="B1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2484,10 +2485,10 @@
       <c r="L30" t="s">
         <v>112</v>
       </c>
-      <c r="M30" s="28" t="s">
+      <c r="M30" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="N30" s="28"/>
+      <c r="N30" s="30"/>
     </row>
     <row r="31" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
@@ -2508,10 +2509,10 @@
       <c r="L31" t="s">
         <v>98</v>
       </c>
-      <c r="M31" s="28" t="s">
+      <c r="M31" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="N31" s="28"/>
+      <c r="N31" s="30"/>
     </row>
     <row r="32" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
@@ -2523,10 +2524,10 @@
       <c r="L32" t="s">
         <v>119</v>
       </c>
-      <c r="M32" s="28" t="s">
+      <c r="M32" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="N32" s="28"/>
+      <c r="N32" s="30"/>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
@@ -2541,19 +2542,19 @@
       <c r="L33" t="s">
         <v>127</v>
       </c>
-      <c r="M33" s="28" t="s">
+      <c r="M33" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="N33" s="28"/>
+      <c r="N33" s="30"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L34" t="s">
         <v>118</v>
       </c>
-      <c r="M34" s="28" t="s">
+      <c r="M34" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="N34" s="28"/>
+      <c r="N34" s="30"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
@@ -2565,19 +2566,19 @@
       <c r="L35" t="s">
         <v>123</v>
       </c>
-      <c r="M35" s="29" t="s">
+      <c r="M35" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="N35" s="29"/>
+      <c r="N35" s="31"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L36" t="s">
         <v>124</v>
       </c>
-      <c r="M36" s="29" t="s">
+      <c r="M36" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="N36" s="29"/>
+      <c r="N36" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2601,77 +2602,78 @@
   <dimension ref="A1:W38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="V20" sqref="V20:W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="22" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
     <col min="4" max="4" width="2.7109375" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" style="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.7109375" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" style="22" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="2.7109375" customWidth="1"/>
-    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2.7109375" customWidth="1"/>
-    <col min="18" max="18" width="2.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="2.7109375" customWidth="1"/>
     <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.42578125" customWidth="1"/>
-    <col min="23" max="23" width="1.140625" customWidth="1"/>
+    <col min="22" max="22" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31"/>
+      <c r="A1" s="33"/>
+      <c r="B1" s="33"/>
       <c r="C1" s="19"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="25" t="s">
+      <c r="A2" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>93</v>
       </c>
       <c r="D2" s="20"/>
-      <c r="E2" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F2" s="25" t="s">
+      <c r="E2" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>64</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>216</v>
       </c>
       <c r="H2" s="20"/>
-      <c r="I2" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="25" t="s">
+      <c r="I2" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="24" t="s">
         <v>64</v>
       </c>
       <c r="K2" s="21" t="s">
         <v>220</v>
       </c>
       <c r="L2" s="20"/>
-      <c r="M2" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N2" s="25" t="s">
+      <c r="M2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N2" s="24" t="s">
         <v>64</v>
       </c>
       <c r="O2" s="21" t="s">
@@ -2681,53 +2683,52 @@
       <c r="Q2" t="s">
         <v>151</v>
       </c>
-      <c r="R2" s="23" t="s">
+      <c r="R2" s="22" t="s">
         <v>64</v>
       </c>
       <c r="T2" s="20"/>
-      <c r="U2" s="24" t="s">
+      <c r="U2" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="V2" s="34" t="s">
+      <c r="V2" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="W2" s="34"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="25" t="s">
+      <c r="A3" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="21" t="s">
         <v>203</v>
       </c>
       <c r="D3" s="20"/>
-      <c r="E3" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="24" t="s">
         <v>65</v>
       </c>
       <c r="G3" s="21" t="s">
         <v>204</v>
       </c>
       <c r="H3" s="20"/>
-      <c r="I3" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J3" s="25" t="s">
+      <c r="I3" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="24" t="s">
         <v>65</v>
       </c>
       <c r="K3" s="21" t="s">
         <v>205</v>
       </c>
       <c r="L3" s="20"/>
-      <c r="M3" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N3" s="25" t="s">
+      <c r="M3" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N3" s="24" t="s">
         <v>65</v>
       </c>
       <c r="O3" s="21" t="s">
@@ -2737,53 +2738,52 @@
       <c r="Q3" t="s">
         <v>151</v>
       </c>
-      <c r="R3" s="23" t="s">
+      <c r="R3" s="22" t="s">
         <v>65</v>
       </c>
       <c r="T3" s="20"/>
-      <c r="U3" s="24" t="s">
+      <c r="U3" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="V3" s="34" t="s">
+      <c r="V3" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="W3" s="34"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="25" t="s">
+      <c r="A4" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>66</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>207</v>
       </c>
       <c r="D4" s="20"/>
-      <c r="E4" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F4" s="25" t="s">
+      <c r="E4" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="24" t="s">
         <v>66</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>208</v>
       </c>
       <c r="H4" s="20"/>
-      <c r="I4" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J4" s="25" t="s">
+      <c r="I4" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="24" t="s">
         <v>66</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>209</v>
       </c>
       <c r="L4" s="20"/>
-      <c r="M4" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N4" s="25" t="s">
+      <c r="M4" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N4" s="24" t="s">
         <v>66</v>
       </c>
       <c r="O4" s="21" t="s">
@@ -2793,78 +2793,78 @@
       <c r="Q4" t="s">
         <v>151</v>
       </c>
-      <c r="R4" s="23" t="s">
+      <c r="R4" s="22" t="s">
         <v>66</v>
       </c>
       <c r="T4" s="20"/>
       <c r="U4" s="2" t="s">
         <v>119</v>
       </c>
+      <c r="V4" s="27"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="25" t="s">
+      <c r="A5" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>67</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>211</v>
       </c>
       <c r="D5" s="20"/>
-      <c r="E5" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="25" t="s">
+      <c r="E5" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="24" t="s">
         <v>67</v>
       </c>
       <c r="G5" s="21" t="s">
         <v>212</v>
       </c>
       <c r="H5" s="20"/>
-      <c r="I5" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J5" s="25" t="s">
+      <c r="I5" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5" s="24" t="s">
         <v>67</v>
       </c>
       <c r="K5" s="21" t="s">
         <v>213</v>
       </c>
       <c r="L5" s="20"/>
-      <c r="M5" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N5" s="25" t="s">
+      <c r="M5" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N5" s="24" t="s">
         <v>67</v>
       </c>
       <c r="O5" s="21" t="s">
         <v>214</v>
       </c>
       <c r="P5" s="20"/>
-      <c r="Q5" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="R5" s="25" t="s">
+      <c r="Q5" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="R5" s="24" t="s">
         <v>67</v>
       </c>
       <c r="S5" s="21" t="s">
         <v>97</v>
       </c>
       <c r="T5" s="20"/>
-      <c r="U5" s="24" t="s">
+      <c r="U5" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="V5" s="34" t="s">
+      <c r="V5" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="W5" s="34"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="25" t="s">
+      <c r="A6" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>68</v>
       </c>
       <c r="C6" s="21" t="s">
@@ -2874,44 +2874,43 @@
       <c r="E6" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="25" t="s">
         <v>68</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="25" t="s">
         <v>68</v>
       </c>
       <c r="L6" s="20"/>
       <c r="M6" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N6" s="26" t="s">
+      <c r="N6" s="25" t="s">
         <v>68</v>
       </c>
       <c r="P6" s="20"/>
       <c r="Q6" t="s">
         <v>151</v>
       </c>
-      <c r="R6" s="23" t="s">
+      <c r="R6" s="22" t="s">
         <v>68</v>
       </c>
       <c r="T6" s="20"/>
-      <c r="U6" s="24" t="s">
+      <c r="U6" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="V6" s="34" t="s">
+      <c r="V6" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="W6" s="34"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="25" t="s">
+      <c r="A7" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>69</v>
       </c>
       <c r="C7" s="21" t="s">
@@ -2921,43 +2920,43 @@
       <c r="E7" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="25" t="s">
         <v>69</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="25" t="s">
         <v>69</v>
       </c>
       <c r="L7" s="20"/>
       <c r="M7" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N7" s="26" t="s">
+      <c r="N7" s="25" t="s">
         <v>69</v>
       </c>
       <c r="P7" s="20"/>
       <c r="Q7" t="s">
         <v>151</v>
       </c>
-      <c r="R7" s="23" t="s">
+      <c r="R7" s="22" t="s">
         <v>69</v>
       </c>
       <c r="T7" s="20"/>
-      <c r="U7" s="24" t="s">
+      <c r="U7" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="V7" s="21" t="s">
+      <c r="V7" s="29" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="25" t="s">
+      <c r="A8" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="24" t="s">
         <v>70</v>
       </c>
       <c r="C8" s="21" t="s">
@@ -2967,24 +2966,24 @@
       <c r="E8" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="25" t="s">
         <v>70</v>
       </c>
       <c r="H8" s="20"/>
-      <c r="I8" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" s="25" t="s">
+      <c r="I8" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="24" t="s">
         <v>70</v>
       </c>
       <c r="K8" s="21" t="s">
         <v>162</v>
       </c>
       <c r="L8" s="20"/>
-      <c r="M8" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N8" s="25" t="s">
+      <c r="M8" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N8" s="24" t="s">
         <v>70</v>
       </c>
       <c r="O8" s="21" t="s">
@@ -2994,23 +2993,22 @@
       <c r="Q8" t="s">
         <v>151</v>
       </c>
-      <c r="R8" s="23" t="s">
+      <c r="R8" s="22" t="s">
         <v>70</v>
       </c>
       <c r="T8" s="20"/>
-      <c r="U8" s="24" t="s">
+      <c r="U8" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="V8" s="29" t="s">
+      <c r="V8" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="W8" s="29"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="25" t="s">
+      <c r="A9" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="21" t="s">
@@ -3020,44 +3018,43 @@
       <c r="E9" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="25" t="s">
         <v>71</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="25" t="s">
         <v>71</v>
       </c>
       <c r="L9" s="20"/>
       <c r="M9" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N9" s="26" t="s">
+      <c r="N9" s="25" t="s">
         <v>71</v>
       </c>
       <c r="P9" s="20"/>
       <c r="Q9" t="s">
         <v>151</v>
       </c>
-      <c r="R9" s="23" t="s">
+      <c r="R9" s="22" t="s">
         <v>71</v>
       </c>
       <c r="T9" s="20"/>
-      <c r="U9" s="24" t="s">
+      <c r="U9" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="V9" s="22" t="s">
+      <c r="V9" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="W9" s="22"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="25" t="s">
+      <c r="A10" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="24" t="s">
         <v>72</v>
       </c>
       <c r="C10" s="21" t="s">
@@ -3067,88 +3064,88 @@
       <c r="E10" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="25" t="s">
         <v>72</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="25" t="s">
         <v>72</v>
       </c>
       <c r="L10" s="20"/>
       <c r="M10" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N10" s="26" t="s">
+      <c r="N10" s="25" t="s">
         <v>72</v>
       </c>
       <c r="P10" s="20"/>
       <c r="Q10" t="s">
         <v>151</v>
       </c>
-      <c r="R10" s="23" t="s">
+      <c r="R10" s="22" t="s">
         <v>72</v>
       </c>
       <c r="T10" s="20"/>
-      <c r="V10" s="32"/>
-      <c r="W10" s="32"/>
+      <c r="V10" s="35"/>
+      <c r="W10" s="35"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="25" t="s">
         <v>73</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="25" t="s">
         <v>73</v>
       </c>
       <c r="L11" s="20"/>
       <c r="M11" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N11" s="26" t="s">
+      <c r="N11" s="25" t="s">
         <v>73</v>
       </c>
       <c r="P11" s="20"/>
       <c r="Q11" t="s">
         <v>151</v>
       </c>
-      <c r="R11" s="23" t="s">
+      <c r="R11" s="22" t="s">
         <v>73</v>
       </c>
       <c r="T11" s="20"/>
-      <c r="V11" s="32"/>
-      <c r="W11" s="32"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="35"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="25" t="s">
+      <c r="A12" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="24" t="s">
         <v>74</v>
       </c>
       <c r="C12" s="21" t="s">
         <v>164</v>
       </c>
       <c r="D12" s="20"/>
-      <c r="E12" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F12" s="25" t="s">
+      <c r="E12" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" s="24" t="s">
         <v>74</v>
       </c>
       <c r="G12" s="21" t="s">
@@ -3158,32 +3155,32 @@
       <c r="I12" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="25" t="s">
         <v>74</v>
       </c>
       <c r="L12" s="20"/>
       <c r="M12" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N12" s="26" t="s">
+      <c r="N12" s="25" t="s">
         <v>74</v>
       </c>
       <c r="P12" s="20"/>
       <c r="Q12" t="s">
         <v>151</v>
       </c>
-      <c r="R12" s="23" t="s">
+      <c r="R12" s="22" t="s">
         <v>74</v>
       </c>
       <c r="T12" s="20"/>
-      <c r="V12" s="32"/>
-      <c r="W12" s="32"/>
+      <c r="V12" s="35"/>
+      <c r="W12" s="35"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="25" t="s">
+      <c r="A13" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>75</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -3193,69 +3190,69 @@
       <c r="E13" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="25" t="s">
         <v>75</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="25" t="s">
         <v>75</v>
       </c>
       <c r="L13" s="20"/>
       <c r="M13" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N13" s="26" t="s">
+      <c r="N13" s="25" t="s">
         <v>75</v>
       </c>
       <c r="P13" s="20"/>
       <c r="Q13" t="s">
         <v>151</v>
       </c>
-      <c r="R13" s="23" t="s">
+      <c r="R13" s="22" t="s">
         <v>75</v>
       </c>
       <c r="T13" s="20"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
+      <c r="V13" s="35"/>
+      <c r="W13" s="35"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="25" t="s">
+      <c r="A14" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>76</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>218</v>
       </c>
       <c r="D14" s="20"/>
-      <c r="E14" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F14" s="25" t="s">
+      <c r="E14" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" s="24" t="s">
         <v>76</v>
       </c>
       <c r="G14" s="21" t="s">
         <v>219</v>
       </c>
       <c r="H14" s="20"/>
-      <c r="I14" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J14" s="25" t="s">
+      <c r="I14" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="24" t="s">
         <v>76</v>
       </c>
       <c r="K14" s="21" t="s">
         <v>222</v>
       </c>
       <c r="L14" s="20"/>
-      <c r="M14" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N14" s="25" t="s">
+      <c r="M14" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N14" s="24" t="s">
         <v>76</v>
       </c>
       <c r="O14" s="21" t="s">
@@ -3265,42 +3262,42 @@
       <c r="Q14" t="s">
         <v>151</v>
       </c>
-      <c r="R14" s="23" t="s">
+      <c r="R14" s="22" t="s">
         <v>76</v>
       </c>
       <c r="T14" s="20"/>
-      <c r="V14" s="32"/>
-      <c r="W14" s="32"/>
+      <c r="V14" s="35"/>
+      <c r="W14" s="35"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="26" t="s">
         <v>77</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" t="s">
         <v>132</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="26" t="s">
         <v>77</v>
       </c>
       <c r="H15" s="20"/>
-      <c r="I15" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J15" s="25" t="s">
+      <c r="I15" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J15" s="24" t="s">
         <v>77</v>
       </c>
       <c r="K15" s="21" t="s">
         <v>229</v>
       </c>
       <c r="L15" s="20"/>
-      <c r="M15" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N15" s="25" t="s">
+      <c r="M15" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N15" s="24" t="s">
         <v>77</v>
       </c>
       <c r="O15" s="21" t="s">
@@ -3310,18 +3307,18 @@
       <c r="Q15" t="s">
         <v>151</v>
       </c>
-      <c r="R15" s="23" t="s">
+      <c r="R15" s="22" t="s">
         <v>77</v>
       </c>
       <c r="T15" s="20"/>
-      <c r="V15" s="32"/>
-      <c r="W15" s="32"/>
+      <c r="V15" s="35"/>
+      <c r="W15" s="35"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="25" t="s">
+      <c r="A16" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>78</v>
       </c>
       <c r="C16" s="21" t="s">
@@ -3331,59 +3328,59 @@
       <c r="E16" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="25" t="s">
         <v>78</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="25" t="s">
         <v>78</v>
       </c>
       <c r="L16" s="20"/>
       <c r="M16" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N16" s="26" t="s">
+      <c r="N16" s="25" t="s">
         <v>78</v>
       </c>
       <c r="P16" s="20"/>
       <c r="Q16" t="s">
         <v>151</v>
       </c>
-      <c r="R16" s="23" t="s">
+      <c r="R16" s="22" t="s">
         <v>78</v>
       </c>
       <c r="T16" s="20"/>
-      <c r="V16" s="32"/>
-      <c r="W16" s="32"/>
+      <c r="V16" s="35"/>
+      <c r="W16" s="35"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="25" t="s">
+      <c r="A17" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>79</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>227</v>
       </c>
       <c r="D17" s="20"/>
-      <c r="E17" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F17" s="25" t="s">
+      <c r="E17" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" s="24" t="s">
         <v>79</v>
       </c>
       <c r="G17" s="21" t="s">
         <v>228</v>
       </c>
       <c r="H17" s="20"/>
-      <c r="I17" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J17" s="25" t="s">
+      <c r="I17" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" s="24" t="s">
         <v>79</v>
       </c>
       <c r="K17" s="21" t="s">
@@ -3393,25 +3390,25 @@
       <c r="M17" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N17" s="26" t="s">
+      <c r="N17" s="25" t="s">
         <v>79</v>
       </c>
       <c r="P17" s="20"/>
       <c r="Q17" t="s">
         <v>151</v>
       </c>
-      <c r="R17" s="23" t="s">
+      <c r="R17" s="22" t="s">
         <v>79</v>
       </c>
       <c r="T17" s="20"/>
-      <c r="V17" s="32"/>
-      <c r="W17" s="32"/>
+      <c r="V17" s="35"/>
+      <c r="W17" s="35"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="25" t="s">
+      <c r="A18" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="24" t="s">
         <v>80</v>
       </c>
       <c r="C18" s="21" t="s">
@@ -3421,69 +3418,69 @@
       <c r="E18" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F18" s="25" t="s">
         <v>80</v>
       </c>
       <c r="H18" s="20"/>
       <c r="I18" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="J18" s="25" t="s">
         <v>80</v>
       </c>
       <c r="L18" s="20"/>
       <c r="M18" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N18" s="26" t="s">
+      <c r="N18" s="25" t="s">
         <v>80</v>
       </c>
       <c r="P18" s="20"/>
       <c r="Q18" t="s">
         <v>151</v>
       </c>
-      <c r="R18" s="23" t="s">
+      <c r="R18" s="22" t="s">
         <v>80</v>
       </c>
       <c r="T18" s="20"/>
-      <c r="V18" s="32"/>
-      <c r="W18" s="32"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="35"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="25" t="s">
+      <c r="A19" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="24" t="s">
         <v>81</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>94</v>
       </c>
       <c r="D19" s="20"/>
-      <c r="E19" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F19" s="25" t="s">
+      <c r="E19" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="24" t="s">
         <v>81</v>
       </c>
       <c r="G19" s="21" t="s">
         <v>135</v>
       </c>
       <c r="H19" s="20"/>
-      <c r="I19" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J19" s="25" t="s">
+      <c r="I19" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" s="24" t="s">
         <v>81</v>
       </c>
       <c r="K19" s="21" t="s">
         <v>167</v>
       </c>
       <c r="L19" s="20"/>
-      <c r="M19" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N19" s="25" t="s">
+      <c r="M19" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N19" s="24" t="s">
         <v>81</v>
       </c>
       <c r="O19" s="21" t="s">
@@ -3493,48 +3490,48 @@
       <c r="Q19" t="s">
         <v>151</v>
       </c>
-      <c r="R19" s="23" t="s">
+      <c r="R19" s="22" t="s">
         <v>81</v>
       </c>
       <c r="T19" s="20"/>
-      <c r="V19" s="32"/>
-      <c r="W19" s="32"/>
+      <c r="V19" s="35"/>
+      <c r="W19" s="35"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="25" t="s">
+      <c r="A20" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="24" t="s">
         <v>82</v>
       </c>
       <c r="C20" s="21" t="s">
         <v>197</v>
       </c>
       <c r="D20" s="20"/>
-      <c r="E20" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F20" s="25" t="s">
+      <c r="E20" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" s="24" t="s">
         <v>82</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>198</v>
       </c>
       <c r="H20" s="20"/>
-      <c r="I20" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J20" s="25" t="s">
+      <c r="I20" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J20" s="24" t="s">
         <v>82</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>199</v>
       </c>
       <c r="L20" s="20"/>
-      <c r="M20" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N20" s="25" t="s">
+      <c r="M20" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N20" s="24" t="s">
         <v>82</v>
       </c>
       <c r="O20" s="21" t="s">
@@ -3544,18 +3541,18 @@
       <c r="Q20" t="s">
         <v>151</v>
       </c>
-      <c r="R20" s="23" t="s">
+      <c r="R20" s="22" t="s">
         <v>82</v>
       </c>
       <c r="T20" s="20"/>
-      <c r="V20" s="32"/>
-      <c r="W20" s="32"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="35"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="25" t="s">
+      <c r="A21" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="24" t="s">
         <v>83</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -3565,24 +3562,24 @@
       <c r="E21" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="25" t="s">
         <v>83</v>
       </c>
       <c r="H21" s="20"/>
-      <c r="I21" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J21" s="25" t="s">
+      <c r="I21" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="24" t="s">
         <v>83</v>
       </c>
       <c r="K21" s="21" t="s">
         <v>168</v>
       </c>
       <c r="L21" s="20"/>
-      <c r="M21" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N21" s="25" t="s">
+      <c r="M21" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N21" s="24" t="s">
         <v>83</v>
       </c>
       <c r="O21" s="21" t="s">
@@ -3592,57 +3589,57 @@
       <c r="Q21" t="s">
         <v>151</v>
       </c>
-      <c r="R21" s="23" t="s">
+      <c r="R21" s="22" t="s">
         <v>83</v>
       </c>
       <c r="T21" s="20"/>
-      <c r="V21" s="32"/>
-      <c r="W21" s="32"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="35"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="25" t="s">
         <v>84</v>
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="25" t="s">
         <v>84</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J22" s="26" t="s">
+      <c r="J22" s="25" t="s">
         <v>84</v>
       </c>
       <c r="L22" s="20"/>
       <c r="M22" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="N22" s="26" t="s">
+      <c r="N22" s="25" t="s">
         <v>84</v>
       </c>
       <c r="P22" s="20"/>
       <c r="Q22" t="s">
         <v>151</v>
       </c>
-      <c r="R22" s="23" t="s">
+      <c r="R22" s="22" t="s">
         <v>84</v>
       </c>
       <c r="T22" s="20"/>
-      <c r="V22" s="32"/>
-      <c r="W22" s="32"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="35"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="25" t="s">
+      <c r="A23" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="24" t="s">
         <v>85</v>
       </c>
       <c r="C23" s="21" t="s">
@@ -3652,24 +3649,24 @@
       <c r="E23" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="25" t="s">
         <v>85</v>
       </c>
       <c r="H23" s="20"/>
-      <c r="I23" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J23" s="25" t="s">
+      <c r="I23" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J23" s="24" t="s">
         <v>85</v>
       </c>
       <c r="K23" s="21" t="s">
         <v>170</v>
       </c>
       <c r="L23" s="20"/>
-      <c r="M23" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N23" s="25" t="s">
+      <c r="M23" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N23" s="24" t="s">
         <v>85</v>
       </c>
       <c r="O23" s="21" t="s">
@@ -3679,28 +3676,28 @@
       <c r="Q23" t="s">
         <v>151</v>
       </c>
-      <c r="R23" s="23" t="s">
+      <c r="R23" s="22" t="s">
         <v>85</v>
       </c>
       <c r="T23" s="20"/>
-      <c r="V23" s="32"/>
-      <c r="W23" s="32"/>
+      <c r="V23" s="35"/>
+      <c r="W23" s="35"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="25" t="s">
+      <c r="A24" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="24" t="s">
         <v>86</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>201</v>
       </c>
       <c r="D24" s="20"/>
-      <c r="E24" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F24" s="25" t="s">
+      <c r="E24" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="24" t="s">
         <v>86</v>
       </c>
       <c r="G24" s="21" t="s">
@@ -3710,120 +3707,120 @@
       <c r="I24" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J24" s="26" t="s">
+      <c r="J24" s="25" t="s">
         <v>86</v>
       </c>
       <c r="L24" s="20"/>
       <c r="M24" t="s">
         <v>134</v>
       </c>
-      <c r="N24" s="23" t="s">
+      <c r="N24" s="22" t="s">
         <v>86</v>
       </c>
       <c r="P24" s="20"/>
       <c r="Q24" t="s">
         <v>151</v>
       </c>
-      <c r="R24" s="23" t="s">
+      <c r="R24" s="22" t="s">
         <v>86</v>
       </c>
       <c r="T24" s="20"/>
-      <c r="V24" s="32"/>
-      <c r="W24" s="32"/>
+      <c r="V24" s="35"/>
+      <c r="W24" s="35"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>87</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F25" s="26" t="s">
+      <c r="F25" s="25" t="s">
         <v>87</v>
       </c>
       <c r="H25" s="20"/>
       <c r="I25" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J25" s="26" t="s">
+      <c r="J25" s="25" t="s">
         <v>87</v>
       </c>
       <c r="L25" s="20"/>
       <c r="M25" t="s">
         <v>134</v>
       </c>
-      <c r="N25" s="23" t="s">
+      <c r="N25" s="22" t="s">
         <v>87</v>
       </c>
       <c r="P25" s="20"/>
       <c r="Q25" t="s">
         <v>151</v>
       </c>
-      <c r="R25" s="23" t="s">
+      <c r="R25" s="22" t="s">
         <v>87</v>
       </c>
       <c r="T25" s="20"/>
-      <c r="V25" s="32"/>
-      <c r="W25" s="32"/>
+      <c r="V25" s="35"/>
+      <c r="W25" s="35"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="25" t="s">
         <v>88</v>
       </c>
       <c r="D26" s="20"/>
       <c r="E26" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="25" t="s">
         <v>88</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J26" s="26" t="s">
+      <c r="J26" s="25" t="s">
         <v>88</v>
       </c>
       <c r="L26" s="20"/>
       <c r="M26" t="s">
         <v>134</v>
       </c>
-      <c r="N26" s="23" t="s">
+      <c r="N26" s="22" t="s">
         <v>88</v>
       </c>
       <c r="P26" s="20"/>
       <c r="Q26" t="s">
         <v>151</v>
       </c>
-      <c r="R26" s="23" t="s">
+      <c r="R26" s="22" t="s">
         <v>88</v>
       </c>
       <c r="T26" s="20"/>
-      <c r="V26" s="32"/>
-      <c r="W26" s="32"/>
+      <c r="V26" s="35"/>
+      <c r="W26" s="35"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="25" t="s">
+      <c r="A27" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="24" t="s">
         <v>89</v>
       </c>
       <c r="C27" s="21" t="s">
         <v>172</v>
       </c>
       <c r="D27" s="20"/>
-      <c r="E27" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F27" s="25" t="s">
+      <c r="E27" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="24" t="s">
         <v>89</v>
       </c>
       <c r="G27" s="21" t="s">
@@ -3833,52 +3830,52 @@
       <c r="I27" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J27" s="26" t="s">
+      <c r="J27" s="25" t="s">
         <v>89</v>
       </c>
       <c r="L27" s="20"/>
       <c r="M27" t="s">
         <v>134</v>
       </c>
-      <c r="N27" s="23" t="s">
+      <c r="N27" s="22" t="s">
         <v>89</v>
       </c>
       <c r="P27" s="20"/>
       <c r="Q27" t="s">
         <v>151</v>
       </c>
-      <c r="R27" s="23" t="s">
+      <c r="R27" s="22" t="s">
         <v>89</v>
       </c>
       <c r="T27" s="20"/>
-      <c r="V27" s="32"/>
-      <c r="W27" s="32"/>
+      <c r="V27" s="35"/>
+      <c r="W27" s="35"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="25" t="s">
+      <c r="A28" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="24" t="s">
         <v>115</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>116</v>
       </c>
       <c r="D28" s="20"/>
-      <c r="E28" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F28" s="25" t="s">
+      <c r="E28" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F28" s="24" t="s">
         <v>137</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>159</v>
       </c>
       <c r="H28" s="20"/>
-      <c r="I28" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J28" s="25" t="s">
+      <c r="I28" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J28" s="24" t="s">
         <v>112</v>
       </c>
       <c r="K28" s="21" t="s">
@@ -3887,30 +3884,30 @@
       <c r="L28" s="20"/>
       <c r="P28" s="20"/>
       <c r="T28" s="20"/>
-      <c r="V28" s="32"/>
-      <c r="W28" s="32"/>
+      <c r="V28" s="35"/>
+      <c r="W28" s="35"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A29" s="24" t="s">
+      <c r="A29" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="24" t="s">
         <v>130</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>131</v>
       </c>
       <c r="D29" s="20"/>
-      <c r="E29" s="33" t="s">
+      <c r="E29" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
       <c r="H29" s="20"/>
-      <c r="I29" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J29" s="25" t="s">
+      <c r="I29" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="24" t="s">
         <v>98</v>
       </c>
       <c r="K29" s="21" t="s">
@@ -3919,34 +3916,34 @@
       <c r="L29" s="20"/>
       <c r="P29" s="20"/>
       <c r="T29" s="20"/>
-      <c r="V29" s="32"/>
-      <c r="W29" s="32"/>
+      <c r="V29" s="35"/>
+      <c r="W29" s="35"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="24" t="s">
         <v>136</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>138</v>
       </c>
       <c r="D30" s="20"/>
-      <c r="E30" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F30" s="25">
+      <c r="E30" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F30" s="24">
         <v>1</v>
       </c>
       <c r="G30" s="21" t="s">
         <v>185</v>
       </c>
       <c r="H30" s="20"/>
-      <c r="I30" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J30" s="25" t="s">
+      <c r="I30" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J30" s="24" t="s">
         <v>119</v>
       </c>
       <c r="K30" s="21" t="s">
@@ -3955,34 +3952,34 @@
       <c r="L30" s="20"/>
       <c r="P30" s="20"/>
       <c r="T30" s="20"/>
-      <c r="V30" s="32"/>
-      <c r="W30" s="32"/>
+      <c r="V30" s="35"/>
+      <c r="W30" s="35"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="25" t="s">
+      <c r="A31" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="24" t="s">
         <v>141</v>
       </c>
       <c r="C31" s="21" t="s">
         <v>143</v>
       </c>
       <c r="D31" s="20"/>
-      <c r="E31" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F31" s="25">
+      <c r="E31" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="24">
         <v>2</v>
       </c>
       <c r="G31" s="21" t="s">
         <v>186</v>
       </c>
       <c r="H31" s="20"/>
-      <c r="I31" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J31" s="25" t="s">
+      <c r="I31" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="24" t="s">
         <v>127</v>
       </c>
       <c r="K31" s="21" t="s">
@@ -3991,34 +3988,34 @@
       <c r="L31" s="20"/>
       <c r="P31" s="20"/>
       <c r="T31" s="20"/>
-      <c r="V31" s="32"/>
-      <c r="W31" s="32"/>
+      <c r="V31" s="35"/>
+      <c r="W31" s="35"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="25" t="s">
+      <c r="A32" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="24" t="s">
         <v>163</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>116</v>
       </c>
       <c r="D32" s="20"/>
-      <c r="E32" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F32" s="25">
+      <c r="E32" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F32" s="24">
         <v>3</v>
       </c>
       <c r="G32" s="21" t="s">
         <v>187</v>
       </c>
       <c r="H32" s="20"/>
-      <c r="I32" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J32" s="25" t="s">
+      <c r="I32" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32" s="24" t="s">
         <v>174</v>
       </c>
       <c r="K32" s="21" t="s">
@@ -4027,27 +4024,27 @@
       <c r="L32" s="20"/>
       <c r="P32" s="20"/>
       <c r="T32" s="20"/>
-      <c r="V32" s="32"/>
-      <c r="W32" s="32"/>
+      <c r="V32" s="35"/>
+      <c r="W32" s="35"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="26"/>
+      <c r="B33" s="25"/>
       <c r="D33" s="20"/>
-      <c r="E33" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F33" s="25">
+      <c r="E33" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F33" s="24">
         <v>4</v>
       </c>
       <c r="G33" s="21" t="s">
         <v>188</v>
       </c>
       <c r="H33" s="20"/>
-      <c r="I33" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J33" s="25" t="s">
+      <c r="I33" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J33" s="24" t="s">
         <v>195</v>
       </c>
       <c r="K33" s="21" t="s">
@@ -4056,34 +4053,34 @@
       <c r="L33" s="20"/>
       <c r="P33" s="20"/>
       <c r="T33" s="20"/>
-      <c r="V33" s="32"/>
-      <c r="W33" s="32"/>
+      <c r="V33" s="35"/>
+      <c r="W33" s="35"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="25" t="s">
+      <c r="A34" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="24" t="s">
         <v>112</v>
       </c>
       <c r="C34" s="21" t="s">
         <v>120</v>
       </c>
       <c r="D34" s="20"/>
-      <c r="E34" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" s="25">
+      <c r="E34" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="24">
         <v>5</v>
       </c>
       <c r="G34" s="21" t="s">
         <v>189</v>
       </c>
       <c r="H34" s="20"/>
-      <c r="I34" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J34" s="25" t="s">
+      <c r="I34" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J34" s="24" t="s">
         <v>137</v>
       </c>
       <c r="K34" s="21" t="s">
@@ -4094,30 +4091,30 @@
       <c r="T34" s="20"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="25" t="s">
+      <c r="A35" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="24" t="s">
         <v>98</v>
       </c>
       <c r="C35" s="21" t="s">
         <v>217</v>
       </c>
       <c r="D35" s="20"/>
-      <c r="E35" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F35" s="25">
+      <c r="E35" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F35" s="24">
         <v>6</v>
       </c>
       <c r="G35" s="21" t="s">
         <v>190</v>
       </c>
       <c r="H35" s="20"/>
-      <c r="I35" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J35" s="25" t="s">
+      <c r="I35" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J35" s="24" t="s">
         <v>175</v>
       </c>
       <c r="K35" s="21" t="s">
@@ -4128,30 +4125,30 @@
       <c r="T35" s="20"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36" s="25" t="s">
+      <c r="A36" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="24" t="s">
         <v>119</v>
       </c>
       <c r="C36" s="21" t="s">
         <v>224</v>
       </c>
       <c r="D36" s="20"/>
-      <c r="E36" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F36" s="25">
+      <c r="E36" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="24">
         <v>7</v>
       </c>
       <c r="G36" s="21" t="s">
         <v>191</v>
       </c>
       <c r="H36" s="20"/>
-      <c r="I36" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="J36" s="25" t="s">
+      <c r="I36" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J36" s="24" t="s">
         <v>176</v>
       </c>
       <c r="K36" s="21" t="s">
@@ -4162,20 +4159,20 @@
       <c r="T36" s="20"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="25" t="s">
+      <c r="A37" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="24" t="s">
         <v>127</v>
       </c>
       <c r="C37" s="21" t="s">
         <v>225</v>
       </c>
       <c r="D37" s="20"/>
-      <c r="E37" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="F37" s="25">
+      <c r="E37" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F37" s="24">
         <v>8</v>
       </c>
       <c r="G37" s="21" t="s">
@@ -4183,16 +4180,16 @@
       </c>
       <c r="H37" s="20"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="26"/>
+      <c r="J37" s="25"/>
       <c r="L37" s="20"/>
       <c r="P37" s="20"/>
       <c r="T37" s="20"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="25" t="s">
+      <c r="A38" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" s="24" t="s">
         <v>174</v>
       </c>
       <c r="C38" s="21" t="s">
@@ -4205,14 +4202,25 @@
       <c r="T38" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="27">
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="V22:W22"/>
     <mergeCell ref="E29:G29"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="V8:W8"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="V5:W5"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="V10:W10"/>
     <mergeCell ref="V11:W11"/>
@@ -4222,22 +4230,6 @@
     <mergeCell ref="V15:W15"/>
     <mergeCell ref="V16:W16"/>
     <mergeCell ref="V17:W17"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="V22:W22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#229 - More work on the new Arena Markers
Added Shortcuts for the new markers, added in Rage and Wrath to the
computeTraits function, fixed a bug with the Markers in actions.py,
added Banish, Rage, and Wrath to the toeknList.

Bumped changed files to 1.12.7.0
</commit_message>
<xml_diff>
--- a/Template/OCTGN - Key Map.xlsx
+++ b/Template/OCTGN - Key Map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="238">
   <si>
     <t>Voltaric</t>
   </si>
@@ -721,6 +721,24 @@
   </si>
   <si>
     <t>Get Rulings/Clarifications for Card</t>
+  </si>
+  <si>
+    <t>Add Wrath Marker</t>
+  </si>
+  <si>
+    <t>Remove Wrath Marker</t>
+  </si>
+  <si>
+    <t>Add Rage Marker</t>
+  </si>
+  <si>
+    <t>Remove Rage Marker</t>
+  </si>
+  <si>
+    <t>Add Banish</t>
+  </si>
+  <si>
+    <t>Remove Banish</t>
   </si>
 </sst>
 </file>
@@ -979,10 +997,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2602,7 +2620,7 @@
   <dimension ref="A1:W38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20:W20"/>
+      <selection activeCell="N9" sqref="M9:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2636,8 +2654,8 @@
       <c r="A1" s="33"/>
       <c r="B1" s="33"/>
       <c r="C1" s="19"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -2878,18 +2896,24 @@
         <v>68</v>
       </c>
       <c r="H6" s="20"/>
-      <c r="I6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J6" s="25" t="s">
+      <c r="I6" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" s="24" t="s">
         <v>68</v>
       </c>
+      <c r="K6" s="21" t="s">
+        <v>234</v>
+      </c>
       <c r="L6" s="20"/>
-      <c r="M6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="N6" s="25" t="s">
+      <c r="M6" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N6" s="24" t="s">
         <v>68</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>235</v>
       </c>
       <c r="P6" s="20"/>
       <c r="Q6" t="s">
@@ -3022,18 +3046,24 @@
         <v>71</v>
       </c>
       <c r="H9" s="20"/>
-      <c r="I9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" s="25" t="s">
+      <c r="I9" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="24" t="s">
         <v>71</v>
       </c>
+      <c r="K9" s="21" t="s">
+        <v>236</v>
+      </c>
       <c r="L9" s="20"/>
-      <c r="M9" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="N9" s="25" t="s">
+      <c r="M9" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N9" s="24" t="s">
         <v>71</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>237</v>
       </c>
       <c r="P9" s="20"/>
       <c r="Q9" t="s">
@@ -3089,8 +3119,8 @@
         <v>72</v>
       </c>
       <c r="T10" s="20"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="34"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -3128,8 +3158,8 @@
         <v>73</v>
       </c>
       <c r="T11" s="20"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="35"/>
+      <c r="V11" s="34"/>
+      <c r="W11" s="34"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
@@ -3173,8 +3203,8 @@
         <v>74</v>
       </c>
       <c r="T12" s="20"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="35"/>
+      <c r="V12" s="34"/>
+      <c r="W12" s="34"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
@@ -3215,8 +3245,8 @@
         <v>75</v>
       </c>
       <c r="T13" s="20"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
+      <c r="V13" s="34"/>
+      <c r="W13" s="34"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
@@ -3266,8 +3296,8 @@
         <v>76</v>
       </c>
       <c r="T14" s="20"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
+      <c r="V14" s="34"/>
+      <c r="W14" s="34"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3311,8 +3341,8 @@
         <v>77</v>
       </c>
       <c r="T15" s="20"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
+      <c r="V15" s="34"/>
+      <c r="W15" s="34"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
@@ -3353,8 +3383,8 @@
         <v>78</v>
       </c>
       <c r="T16" s="20"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
+      <c r="V16" s="34"/>
+      <c r="W16" s="34"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
@@ -3401,8 +3431,8 @@
         <v>79</v>
       </c>
       <c r="T17" s="20"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
+      <c r="V17" s="34"/>
+      <c r="W17" s="34"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
@@ -3443,8 +3473,8 @@
         <v>80</v>
       </c>
       <c r="T18" s="20"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
+      <c r="V18" s="34"/>
+      <c r="W18" s="34"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
@@ -3494,8 +3524,8 @@
         <v>81</v>
       </c>
       <c r="T19" s="20"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="35"/>
+      <c r="V19" s="34"/>
+      <c r="W19" s="34"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
@@ -3545,8 +3575,8 @@
         <v>82</v>
       </c>
       <c r="T20" s="20"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35"/>
+      <c r="V20" s="34"/>
+      <c r="W20" s="34"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
@@ -3593,8 +3623,8 @@
         <v>83</v>
       </c>
       <c r="T21" s="20"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="35"/>
+      <c r="V21" s="34"/>
+      <c r="W21" s="34"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -3632,8 +3662,8 @@
         <v>84</v>
       </c>
       <c r="T22" s="20"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
+      <c r="V22" s="34"/>
+      <c r="W22" s="34"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
@@ -3680,8 +3710,8 @@
         <v>85</v>
       </c>
       <c r="T23" s="20"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
+      <c r="V23" s="34"/>
+      <c r="W23" s="34"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
@@ -3704,18 +3734,24 @@
         <v>202</v>
       </c>
       <c r="H24" s="20"/>
-      <c r="I24" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J24" s="25" t="s">
+      <c r="I24" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" s="24" t="s">
         <v>86</v>
       </c>
+      <c r="K24" s="21" t="s">
+        <v>232</v>
+      </c>
       <c r="L24" s="20"/>
-      <c r="M24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N24" s="22" t="s">
+      <c r="M24" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N24" s="24" t="s">
         <v>86</v>
+      </c>
+      <c r="O24" s="21" t="s">
+        <v>233</v>
       </c>
       <c r="P24" s="20"/>
       <c r="Q24" t="s">
@@ -3725,8 +3761,8 @@
         <v>86</v>
       </c>
       <c r="T24" s="20"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="35"/>
+      <c r="V24" s="34"/>
+      <c r="W24" s="34"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -3764,8 +3800,8 @@
         <v>87</v>
       </c>
       <c r="T25" s="20"/>
-      <c r="V25" s="35"/>
-      <c r="W25" s="35"/>
+      <c r="V25" s="34"/>
+      <c r="W25" s="34"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -3803,8 +3839,8 @@
         <v>88</v>
       </c>
       <c r="T26" s="20"/>
-      <c r="V26" s="35"/>
-      <c r="W26" s="35"/>
+      <c r="V26" s="34"/>
+      <c r="W26" s="34"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
@@ -3848,8 +3884,8 @@
         <v>89</v>
       </c>
       <c r="T27" s="20"/>
-      <c r="V27" s="35"/>
-      <c r="W27" s="35"/>
+      <c r="V27" s="34"/>
+      <c r="W27" s="34"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
@@ -3884,8 +3920,8 @@
       <c r="L28" s="20"/>
       <c r="P28" s="20"/>
       <c r="T28" s="20"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="35"/>
+      <c r="V28" s="34"/>
+      <c r="W28" s="34"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
@@ -3898,11 +3934,11 @@
         <v>131</v>
       </c>
       <c r="D29" s="20"/>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
       <c r="H29" s="20"/>
       <c r="I29" s="23" t="s">
         <v>90</v>
@@ -3916,8 +3952,8 @@
       <c r="L29" s="20"/>
       <c r="P29" s="20"/>
       <c r="T29" s="20"/>
-      <c r="V29" s="35"/>
-      <c r="W29" s="35"/>
+      <c r="V29" s="34"/>
+      <c r="W29" s="34"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
@@ -3952,8 +3988,8 @@
       <c r="L30" s="20"/>
       <c r="P30" s="20"/>
       <c r="T30" s="20"/>
-      <c r="V30" s="35"/>
-      <c r="W30" s="35"/>
+      <c r="V30" s="34"/>
+      <c r="W30" s="34"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
@@ -3988,8 +4024,8 @@
       <c r="L31" s="20"/>
       <c r="P31" s="20"/>
       <c r="T31" s="20"/>
-      <c r="V31" s="35"/>
-      <c r="W31" s="35"/>
+      <c r="V31" s="34"/>
+      <c r="W31" s="34"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
@@ -4024,8 +4060,8 @@
       <c r="L32" s="20"/>
       <c r="P32" s="20"/>
       <c r="T32" s="20"/>
-      <c r="V32" s="35"/>
-      <c r="W32" s="35"/>
+      <c r="V32" s="34"/>
+      <c r="W32" s="34"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -4053,8 +4089,8 @@
       <c r="L33" s="20"/>
       <c r="P33" s="20"/>
       <c r="T33" s="20"/>
-      <c r="V33" s="35"/>
-      <c r="W33" s="35"/>
+      <c r="V33" s="34"/>
+      <c r="W33" s="34"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
@@ -4203,22 +4239,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="V22:W22"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="V1:W1"/>
@@ -4230,6 +4250,22 @@
     <mergeCell ref="V15:W15"/>
     <mergeCell ref="V16:W16"/>
     <mergeCell ref="V17:W17"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V29:W29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Shortcuts for the new markers, added in Rage and Wrath to the computeTraits function, fixed a bug with the Markers in actions.py, added Banish, Rage, and Wrath to the toeknList.
Bumped changed files to 1.12.7.0

Conflicts:
	GameDatabase/9acef3d0-efa8-4d3f-a10c-54812baecdda/definition.xml
</commit_message>
<xml_diff>
--- a/Template/OCTGN - Key Map.xlsx
+++ b/Template/OCTGN - Key Map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="238">
   <si>
     <t>Voltaric</t>
   </si>
@@ -721,6 +721,24 @@
   </si>
   <si>
     <t>Get Rulings/Clarifications for Card</t>
+  </si>
+  <si>
+    <t>Add Wrath Marker</t>
+  </si>
+  <si>
+    <t>Remove Wrath Marker</t>
+  </si>
+  <si>
+    <t>Add Rage Marker</t>
+  </si>
+  <si>
+    <t>Remove Rage Marker</t>
+  </si>
+  <si>
+    <t>Add Banish</t>
+  </si>
+  <si>
+    <t>Remove Banish</t>
   </si>
 </sst>
 </file>
@@ -979,10 +997,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2602,7 +2620,7 @@
   <dimension ref="A1:W38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20:W20"/>
+      <selection activeCell="N9" sqref="M9:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2636,8 +2654,8 @@
       <c r="A1" s="33"/>
       <c r="B1" s="33"/>
       <c r="C1" s="19"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -2878,18 +2896,24 @@
         <v>68</v>
       </c>
       <c r="H6" s="20"/>
-      <c r="I6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J6" s="25" t="s">
+      <c r="I6" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" s="24" t="s">
         <v>68</v>
       </c>
+      <c r="K6" s="21" t="s">
+        <v>234</v>
+      </c>
       <c r="L6" s="20"/>
-      <c r="M6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="N6" s="25" t="s">
+      <c r="M6" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N6" s="24" t="s">
         <v>68</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>235</v>
       </c>
       <c r="P6" s="20"/>
       <c r="Q6" t="s">
@@ -3022,18 +3046,24 @@
         <v>71</v>
       </c>
       <c r="H9" s="20"/>
-      <c r="I9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" s="25" t="s">
+      <c r="I9" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="24" t="s">
         <v>71</v>
       </c>
+      <c r="K9" s="21" t="s">
+        <v>236</v>
+      </c>
       <c r="L9" s="20"/>
-      <c r="M9" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="N9" s="25" t="s">
+      <c r="M9" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N9" s="24" t="s">
         <v>71</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>237</v>
       </c>
       <c r="P9" s="20"/>
       <c r="Q9" t="s">
@@ -3089,8 +3119,8 @@
         <v>72</v>
       </c>
       <c r="T10" s="20"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="34"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -3128,8 +3158,8 @@
         <v>73</v>
       </c>
       <c r="T11" s="20"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="35"/>
+      <c r="V11" s="34"/>
+      <c r="W11" s="34"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
@@ -3173,8 +3203,8 @@
         <v>74</v>
       </c>
       <c r="T12" s="20"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="35"/>
+      <c r="V12" s="34"/>
+      <c r="W12" s="34"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
@@ -3215,8 +3245,8 @@
         <v>75</v>
       </c>
       <c r="T13" s="20"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
+      <c r="V13" s="34"/>
+      <c r="W13" s="34"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
@@ -3266,8 +3296,8 @@
         <v>76</v>
       </c>
       <c r="T14" s="20"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
+      <c r="V14" s="34"/>
+      <c r="W14" s="34"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3311,8 +3341,8 @@
         <v>77</v>
       </c>
       <c r="T15" s="20"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
+      <c r="V15" s="34"/>
+      <c r="W15" s="34"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
@@ -3353,8 +3383,8 @@
         <v>78</v>
       </c>
       <c r="T16" s="20"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
+      <c r="V16" s="34"/>
+      <c r="W16" s="34"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
@@ -3401,8 +3431,8 @@
         <v>79</v>
       </c>
       <c r="T17" s="20"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
+      <c r="V17" s="34"/>
+      <c r="W17" s="34"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
@@ -3443,8 +3473,8 @@
         <v>80</v>
       </c>
       <c r="T18" s="20"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
+      <c r="V18" s="34"/>
+      <c r="W18" s="34"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
@@ -3494,8 +3524,8 @@
         <v>81</v>
       </c>
       <c r="T19" s="20"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="35"/>
+      <c r="V19" s="34"/>
+      <c r="W19" s="34"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
@@ -3545,8 +3575,8 @@
         <v>82</v>
       </c>
       <c r="T20" s="20"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35"/>
+      <c r="V20" s="34"/>
+      <c r="W20" s="34"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
@@ -3593,8 +3623,8 @@
         <v>83</v>
       </c>
       <c r="T21" s="20"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="35"/>
+      <c r="V21" s="34"/>
+      <c r="W21" s="34"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -3632,8 +3662,8 @@
         <v>84</v>
       </c>
       <c r="T22" s="20"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
+      <c r="V22" s="34"/>
+      <c r="W22" s="34"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
@@ -3680,8 +3710,8 @@
         <v>85</v>
       </c>
       <c r="T23" s="20"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
+      <c r="V23" s="34"/>
+      <c r="W23" s="34"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
@@ -3704,18 +3734,24 @@
         <v>202</v>
       </c>
       <c r="H24" s="20"/>
-      <c r="I24" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J24" s="25" t="s">
+      <c r="I24" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" s="24" t="s">
         <v>86</v>
       </c>
+      <c r="K24" s="21" t="s">
+        <v>232</v>
+      </c>
       <c r="L24" s="20"/>
-      <c r="M24" t="s">
-        <v>134</v>
-      </c>
-      <c r="N24" s="22" t="s">
+      <c r="M24" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N24" s="24" t="s">
         <v>86</v>
+      </c>
+      <c r="O24" s="21" t="s">
+        <v>233</v>
       </c>
       <c r="P24" s="20"/>
       <c r="Q24" t="s">
@@ -3725,8 +3761,8 @@
         <v>86</v>
       </c>
       <c r="T24" s="20"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="35"/>
+      <c r="V24" s="34"/>
+      <c r="W24" s="34"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -3764,8 +3800,8 @@
         <v>87</v>
       </c>
       <c r="T25" s="20"/>
-      <c r="V25" s="35"/>
-      <c r="W25" s="35"/>
+      <c r="V25" s="34"/>
+      <c r="W25" s="34"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -3803,8 +3839,8 @@
         <v>88</v>
       </c>
       <c r="T26" s="20"/>
-      <c r="V26" s="35"/>
-      <c r="W26" s="35"/>
+      <c r="V26" s="34"/>
+      <c r="W26" s="34"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
@@ -3848,8 +3884,8 @@
         <v>89</v>
       </c>
       <c r="T27" s="20"/>
-      <c r="V27" s="35"/>
-      <c r="W27" s="35"/>
+      <c r="V27" s="34"/>
+      <c r="W27" s="34"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
@@ -3884,8 +3920,8 @@
       <c r="L28" s="20"/>
       <c r="P28" s="20"/>
       <c r="T28" s="20"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="35"/>
+      <c r="V28" s="34"/>
+      <c r="W28" s="34"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
@@ -3898,11 +3934,11 @@
         <v>131</v>
       </c>
       <c r="D29" s="20"/>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
       <c r="H29" s="20"/>
       <c r="I29" s="23" t="s">
         <v>90</v>
@@ -3916,8 +3952,8 @@
       <c r="L29" s="20"/>
       <c r="P29" s="20"/>
       <c r="T29" s="20"/>
-      <c r="V29" s="35"/>
-      <c r="W29" s="35"/>
+      <c r="V29" s="34"/>
+      <c r="W29" s="34"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
@@ -3952,8 +3988,8 @@
       <c r="L30" s="20"/>
       <c r="P30" s="20"/>
       <c r="T30" s="20"/>
-      <c r="V30" s="35"/>
-      <c r="W30" s="35"/>
+      <c r="V30" s="34"/>
+      <c r="W30" s="34"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
@@ -3988,8 +4024,8 @@
       <c r="L31" s="20"/>
       <c r="P31" s="20"/>
       <c r="T31" s="20"/>
-      <c r="V31" s="35"/>
-      <c r="W31" s="35"/>
+      <c r="V31" s="34"/>
+      <c r="W31" s="34"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
@@ -4024,8 +4060,8 @@
       <c r="L32" s="20"/>
       <c r="P32" s="20"/>
       <c r="T32" s="20"/>
-      <c r="V32" s="35"/>
-      <c r="W32" s="35"/>
+      <c r="V32" s="34"/>
+      <c r="W32" s="34"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -4053,8 +4089,8 @@
       <c r="L33" s="20"/>
       <c r="P33" s="20"/>
       <c r="T33" s="20"/>
-      <c r="V33" s="35"/>
-      <c r="W33" s="35"/>
+      <c r="V33" s="34"/>
+      <c r="W33" s="34"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
@@ -4203,22 +4239,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="V19:W19"/>
-    <mergeCell ref="V20:W20"/>
-    <mergeCell ref="V21:W21"/>
-    <mergeCell ref="V22:W22"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="V1:W1"/>
@@ -4230,6 +4250,22 @@
     <mergeCell ref="V15:W15"/>
     <mergeCell ref="V16:W16"/>
     <mergeCell ref="V17:W17"/>
+    <mergeCell ref="V18:W18"/>
+    <mergeCell ref="V19:W19"/>
+    <mergeCell ref="V20:W20"/>
+    <mergeCell ref="V21:W21"/>
+    <mergeCell ref="V22:W22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V29:W29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#229 - adding in the Gate to Hell Markers
Automated the Placement of the Gate Closed marker as well as the ability
to toggle the marker to Gate Opened
#229 - fixed shortcut names for new Arena Markers
#233 - Dice Tower and other Promos added in
</commit_message>
<xml_diff>
--- a/Template/OCTGN - Key Map.xlsx
+++ b/Template/OCTGN - Key Map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="239">
   <si>
     <t>Voltaric</t>
   </si>
@@ -739,6 +739,9 @@
   </si>
   <si>
     <t>Remove Banish</t>
+  </si>
+  <si>
+    <t>Toggle Gate to Hell Marker</t>
   </si>
 </sst>
 </file>
@@ -997,10 +1000,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2620,7 +2623,7 @@
   <dimension ref="A1:W38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N9" sqref="M9:N9"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2654,8 +2657,8 @@
       <c r="A1" s="33"/>
       <c r="B1" s="33"/>
       <c r="C1" s="19"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -2987,11 +2990,14 @@
         <v>111</v>
       </c>
       <c r="D8" s="20"/>
-      <c r="E8" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F8" s="25" t="s">
+      <c r="E8" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="24" t="s">
         <v>70</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>238</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="23" t="s">
@@ -3119,8 +3125,8 @@
         <v>72</v>
       </c>
       <c r="T10" s="20"/>
-      <c r="V10" s="34"/>
-      <c r="W10" s="34"/>
+      <c r="V10" s="35"/>
+      <c r="W10" s="35"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -3158,8 +3164,8 @@
         <v>73</v>
       </c>
       <c r="T11" s="20"/>
-      <c r="V11" s="34"/>
-      <c r="W11" s="34"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="35"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
@@ -3203,8 +3209,8 @@
         <v>74</v>
       </c>
       <c r="T12" s="20"/>
-      <c r="V12" s="34"/>
-      <c r="W12" s="34"/>
+      <c r="V12" s="35"/>
+      <c r="W12" s="35"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
@@ -3245,8 +3251,8 @@
         <v>75</v>
       </c>
       <c r="T13" s="20"/>
-      <c r="V13" s="34"/>
-      <c r="W13" s="34"/>
+      <c r="V13" s="35"/>
+      <c r="W13" s="35"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
@@ -3296,8 +3302,8 @@
         <v>76</v>
       </c>
       <c r="T14" s="20"/>
-      <c r="V14" s="34"/>
-      <c r="W14" s="34"/>
+      <c r="V14" s="35"/>
+      <c r="W14" s="35"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3341,8 +3347,8 @@
         <v>77</v>
       </c>
       <c r="T15" s="20"/>
-      <c r="V15" s="34"/>
-      <c r="W15" s="34"/>
+      <c r="V15" s="35"/>
+      <c r="W15" s="35"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
@@ -3383,8 +3389,8 @@
         <v>78</v>
       </c>
       <c r="T16" s="20"/>
-      <c r="V16" s="34"/>
-      <c r="W16" s="34"/>
+      <c r="V16" s="35"/>
+      <c r="W16" s="35"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
@@ -3431,8 +3437,8 @@
         <v>79</v>
       </c>
       <c r="T17" s="20"/>
-      <c r="V17" s="34"/>
-      <c r="W17" s="34"/>
+      <c r="V17" s="35"/>
+      <c r="W17" s="35"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
@@ -3473,8 +3479,8 @@
         <v>80</v>
       </c>
       <c r="T18" s="20"/>
-      <c r="V18" s="34"/>
-      <c r="W18" s="34"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="35"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
@@ -3524,8 +3530,8 @@
         <v>81</v>
       </c>
       <c r="T19" s="20"/>
-      <c r="V19" s="34"/>
-      <c r="W19" s="34"/>
+      <c r="V19" s="35"/>
+      <c r="W19" s="35"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
@@ -3575,8 +3581,8 @@
         <v>82</v>
       </c>
       <c r="T20" s="20"/>
-      <c r="V20" s="34"/>
-      <c r="W20" s="34"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="35"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
@@ -3623,8 +3629,8 @@
         <v>83</v>
       </c>
       <c r="T21" s="20"/>
-      <c r="V21" s="34"/>
-      <c r="W21" s="34"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="35"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -3662,8 +3668,8 @@
         <v>84</v>
       </c>
       <c r="T22" s="20"/>
-      <c r="V22" s="34"/>
-      <c r="W22" s="34"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="35"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
@@ -3710,8 +3716,8 @@
         <v>85</v>
       </c>
       <c r="T23" s="20"/>
-      <c r="V23" s="34"/>
-      <c r="W23" s="34"/>
+      <c r="V23" s="35"/>
+      <c r="W23" s="35"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
@@ -3761,8 +3767,8 @@
         <v>86</v>
       </c>
       <c r="T24" s="20"/>
-      <c r="V24" s="34"/>
-      <c r="W24" s="34"/>
+      <c r="V24" s="35"/>
+      <c r="W24" s="35"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -3800,8 +3806,8 @@
         <v>87</v>
       </c>
       <c r="T25" s="20"/>
-      <c r="V25" s="34"/>
-      <c r="W25" s="34"/>
+      <c r="V25" s="35"/>
+      <c r="W25" s="35"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -3839,8 +3845,8 @@
         <v>88</v>
       </c>
       <c r="T26" s="20"/>
-      <c r="V26" s="34"/>
-      <c r="W26" s="34"/>
+      <c r="V26" s="35"/>
+      <c r="W26" s="35"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
@@ -3884,8 +3890,8 @@
         <v>89</v>
       </c>
       <c r="T27" s="20"/>
-      <c r="V27" s="34"/>
-      <c r="W27" s="34"/>
+      <c r="V27" s="35"/>
+      <c r="W27" s="35"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
@@ -3920,8 +3926,8 @@
       <c r="L28" s="20"/>
       <c r="P28" s="20"/>
       <c r="T28" s="20"/>
-      <c r="V28" s="34"/>
-      <c r="W28" s="34"/>
+      <c r="V28" s="35"/>
+      <c r="W28" s="35"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
@@ -3934,11 +3940,11 @@
         <v>131</v>
       </c>
       <c r="D29" s="20"/>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
       <c r="H29" s="20"/>
       <c r="I29" s="23" t="s">
         <v>90</v>
@@ -3952,8 +3958,8 @@
       <c r="L29" s="20"/>
       <c r="P29" s="20"/>
       <c r="T29" s="20"/>
-      <c r="V29" s="34"/>
-      <c r="W29" s="34"/>
+      <c r="V29" s="35"/>
+      <c r="W29" s="35"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
@@ -3988,8 +3994,8 @@
       <c r="L30" s="20"/>
       <c r="P30" s="20"/>
       <c r="T30" s="20"/>
-      <c r="V30" s="34"/>
-      <c r="W30" s="34"/>
+      <c r="V30" s="35"/>
+      <c r="W30" s="35"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
@@ -4024,8 +4030,8 @@
       <c r="L31" s="20"/>
       <c r="P31" s="20"/>
       <c r="T31" s="20"/>
-      <c r="V31" s="34"/>
-      <c r="W31" s="34"/>
+      <c r="V31" s="35"/>
+      <c r="W31" s="35"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
@@ -4060,8 +4066,8 @@
       <c r="L32" s="20"/>
       <c r="P32" s="20"/>
       <c r="T32" s="20"/>
-      <c r="V32" s="34"/>
-      <c r="W32" s="34"/>
+      <c r="V32" s="35"/>
+      <c r="W32" s="35"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -4089,8 +4095,8 @@
       <c r="L33" s="20"/>
       <c r="P33" s="20"/>
       <c r="T33" s="20"/>
-      <c r="V33" s="34"/>
-      <c r="W33" s="34"/>
+      <c r="V33" s="35"/>
+      <c r="W33" s="35"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
@@ -4239,6 +4245,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V32:W32"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="V1:W1"/>
@@ -4255,17 +4272,6 @@
     <mergeCell ref="V20:W20"/>
     <mergeCell ref="V21:W21"/>
     <mergeCell ref="V22:W22"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#255 - More Work on Control Markers
#249 - Updated Purple ini Marker with new shade of purple
</commit_message>
<xml_diff>
--- a/Template/OCTGN - Key Map.xlsx
+++ b/Template/OCTGN - Key Map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="241">
   <si>
     <t>Voltaric</t>
   </si>
@@ -742,6 +742,12 @@
   </si>
   <si>
     <t>Toggle Gate to Hell Marker</t>
+  </si>
+  <si>
+    <t>Add Control Marker</t>
+  </si>
+  <si>
+    <t>Remove Control Marker</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1006,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2623,7 +2629,7 @@
   <dimension ref="A1:W38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2657,8 +2663,8 @@
       <c r="A1" s="33"/>
       <c r="B1" s="33"/>
       <c r="C1" s="19"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -3125,8 +3131,8 @@
         <v>72</v>
       </c>
       <c r="T10" s="20"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="34"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -3164,8 +3170,8 @@
         <v>73</v>
       </c>
       <c r="T11" s="20"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="35"/>
+      <c r="V11" s="34"/>
+      <c r="W11" s="34"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
@@ -3209,8 +3215,8 @@
         <v>74</v>
       </c>
       <c r="T12" s="20"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="35"/>
+      <c r="V12" s="34"/>
+      <c r="W12" s="34"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
@@ -3251,8 +3257,8 @@
         <v>75</v>
       </c>
       <c r="T13" s="20"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
+      <c r="V13" s="34"/>
+      <c r="W13" s="34"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
@@ -3302,8 +3308,8 @@
         <v>76</v>
       </c>
       <c r="T14" s="20"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
+      <c r="V14" s="34"/>
+      <c r="W14" s="34"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3347,8 +3353,8 @@
         <v>77</v>
       </c>
       <c r="T15" s="20"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
+      <c r="V15" s="34"/>
+      <c r="W15" s="34"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
@@ -3368,18 +3374,24 @@
         <v>78</v>
       </c>
       <c r="H16" s="20"/>
-      <c r="I16" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J16" s="25" t="s">
+      <c r="I16" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" s="24" t="s">
         <v>78</v>
       </c>
+      <c r="K16" s="21" t="s">
+        <v>239</v>
+      </c>
       <c r="L16" s="20"/>
-      <c r="M16" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="N16" s="25" t="s">
+      <c r="M16" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="N16" s="24" t="s">
         <v>78</v>
+      </c>
+      <c r="O16" s="21" t="s">
+        <v>240</v>
       </c>
       <c r="P16" s="20"/>
       <c r="Q16" t="s">
@@ -3389,8 +3401,8 @@
         <v>78</v>
       </c>
       <c r="T16" s="20"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
+      <c r="V16" s="34"/>
+      <c r="W16" s="34"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
@@ -3437,8 +3449,8 @@
         <v>79</v>
       </c>
       <c r="T17" s="20"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
+      <c r="V17" s="34"/>
+      <c r="W17" s="34"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
@@ -3479,8 +3491,8 @@
         <v>80</v>
       </c>
       <c r="T18" s="20"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
+      <c r="V18" s="34"/>
+      <c r="W18" s="34"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
@@ -3530,8 +3542,8 @@
         <v>81</v>
       </c>
       <c r="T19" s="20"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="35"/>
+      <c r="V19" s="34"/>
+      <c r="W19" s="34"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
@@ -3581,8 +3593,8 @@
         <v>82</v>
       </c>
       <c r="T20" s="20"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35"/>
+      <c r="V20" s="34"/>
+      <c r="W20" s="34"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
@@ -3629,8 +3641,8 @@
         <v>83</v>
       </c>
       <c r="T21" s="20"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="35"/>
+      <c r="V21" s="34"/>
+      <c r="W21" s="34"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -3668,8 +3680,8 @@
         <v>84</v>
       </c>
       <c r="T22" s="20"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
+      <c r="V22" s="34"/>
+      <c r="W22" s="34"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
@@ -3716,8 +3728,8 @@
         <v>85</v>
       </c>
       <c r="T23" s="20"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
+      <c r="V23" s="34"/>
+      <c r="W23" s="34"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
@@ -3767,8 +3779,8 @@
         <v>86</v>
       </c>
       <c r="T24" s="20"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="35"/>
+      <c r="V24" s="34"/>
+      <c r="W24" s="34"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -3806,8 +3818,8 @@
         <v>87</v>
       </c>
       <c r="T25" s="20"/>
-      <c r="V25" s="35"/>
-      <c r="W25" s="35"/>
+      <c r="V25" s="34"/>
+      <c r="W25" s="34"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -3845,8 +3857,8 @@
         <v>88</v>
       </c>
       <c r="T26" s="20"/>
-      <c r="V26" s="35"/>
-      <c r="W26" s="35"/>
+      <c r="V26" s="34"/>
+      <c r="W26" s="34"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
@@ -3890,8 +3902,8 @@
         <v>89</v>
       </c>
       <c r="T27" s="20"/>
-      <c r="V27" s="35"/>
-      <c r="W27" s="35"/>
+      <c r="V27" s="34"/>
+      <c r="W27" s="34"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
@@ -3926,8 +3938,8 @@
       <c r="L28" s="20"/>
       <c r="P28" s="20"/>
       <c r="T28" s="20"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="35"/>
+      <c r="V28" s="34"/>
+      <c r="W28" s="34"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
@@ -3940,11 +3952,11 @@
         <v>131</v>
       </c>
       <c r="D29" s="20"/>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="35" t="s">
         <v>184</v>
       </c>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
       <c r="H29" s="20"/>
       <c r="I29" s="23" t="s">
         <v>90</v>
@@ -3958,8 +3970,8 @@
       <c r="L29" s="20"/>
       <c r="P29" s="20"/>
       <c r="T29" s="20"/>
-      <c r="V29" s="35"/>
-      <c r="W29" s="35"/>
+      <c r="V29" s="34"/>
+      <c r="W29" s="34"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
@@ -3994,8 +4006,8 @@
       <c r="L30" s="20"/>
       <c r="P30" s="20"/>
       <c r="T30" s="20"/>
-      <c r="V30" s="35"/>
-      <c r="W30" s="35"/>
+      <c r="V30" s="34"/>
+      <c r="W30" s="34"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
@@ -4030,8 +4042,8 @@
       <c r="L31" s="20"/>
       <c r="P31" s="20"/>
       <c r="T31" s="20"/>
-      <c r="V31" s="35"/>
-      <c r="W31" s="35"/>
+      <c r="V31" s="34"/>
+      <c r="W31" s="34"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
@@ -4066,8 +4078,8 @@
       <c r="L32" s="20"/>
       <c r="P32" s="20"/>
       <c r="T32" s="20"/>
-      <c r="V32" s="35"/>
-      <c r="W32" s="35"/>
+      <c r="V32" s="34"/>
+      <c r="W32" s="34"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -4095,8 +4107,8 @@
       <c r="L33" s="20"/>
       <c r="P33" s="20"/>
       <c r="T33" s="20"/>
-      <c r="V33" s="35"/>
-      <c r="W33" s="35"/>
+      <c r="V33" s="34"/>
+      <c r="W33" s="34"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
@@ -4245,17 +4257,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="V1:W1"/>
@@ -4272,6 +4273,17 @@
     <mergeCell ref="V20:W20"/>
     <mergeCell ref="V21:W21"/>
     <mergeCell ref="V22:W22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V29:W29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
#275 - added in more Academy centric targets
#290 - attempt to automate Wounded Prey against (friendly) scenario
Sslak's
#324  - automate Lightning Raptor's attack and counterstrike
#324 - add in timing prompts to reveal Academy Enchantments
#285 - more fixes to card data to help with the Automation process
#324 - add shortcut for Charge Tokens, Wish Tokens, and Stagger Markers
#324 - Automate Packleader's Cowl
#275 & #292 -  fixed "minor creature" detection formula with the change
to the new API
#341 - Mages Level 5 and above now roll one additional attack die with
Academy Weapons
#324 - Automate Slavorg's casting discount (not complete)
#340 - fixed for figuring out creature levels (int to eval)
#283 - added in some chat text to ToLs attack
#190 - Stranglevine now (appropriately) gains life with each Crush Token

Tuned Mage Colors for better/eaisier viewing in the Chat Window
</commit_message>
<xml_diff>
--- a/Template/OCTGN - Key Map.xlsx
+++ b/Template/OCTGN - Key Map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="243">
   <si>
     <t>Voltaric</t>
   </si>
@@ -745,6 +745,15 @@
   </si>
   <si>
     <t>Remove Retribution Token</t>
+  </si>
+  <si>
+    <t>Add Stagger</t>
+  </si>
+  <si>
+    <t>Add Wish Token</t>
+  </si>
+  <si>
+    <t>Add Charge Token</t>
   </si>
 </sst>
 </file>
@@ -2623,7 +2632,7 @@
   <dimension ref="A1:W38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2811,11 +2820,14 @@
         <v>210</v>
       </c>
       <c r="P4" s="20"/>
-      <c r="Q4" t="s">
-        <v>151</v>
-      </c>
-      <c r="R4" s="22" t="s">
+      <c r="Q4" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="R4" s="24" t="s">
         <v>66</v>
+      </c>
+      <c r="S4" s="21" t="s">
+        <v>242</v>
       </c>
       <c r="T4" s="20"/>
       <c r="U4" s="2" t="s">
@@ -3577,11 +3589,14 @@
         <v>200</v>
       </c>
       <c r="P20" s="20"/>
-      <c r="Q20" t="s">
-        <v>151</v>
-      </c>
-      <c r="R20" s="22" t="s">
+      <c r="Q20" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="R20" s="24" t="s">
         <v>82</v>
+      </c>
+      <c r="S20" s="21" t="s">
+        <v>240</v>
       </c>
       <c r="T20" s="20"/>
       <c r="V20" s="34"/>
@@ -3763,11 +3778,14 @@
         <v>233</v>
       </c>
       <c r="P24" s="20"/>
-      <c r="Q24" t="s">
-        <v>151</v>
-      </c>
-      <c r="R24" s="22" t="s">
+      <c r="Q24" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="R24" s="24" t="s">
         <v>86</v>
+      </c>
+      <c r="S24" s="21" t="s">
+        <v>241</v>
       </c>
       <c r="T24" s="20"/>
       <c r="V24" s="34"/>

</xml_diff>

<commit_message>
Updated Key Mapping SpreadSheet
</commit_message>
<xml_diff>
--- a/Template/OCTGN - Key Map.xlsx
+++ b/Template/OCTGN - Key Map.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="245">
   <si>
     <t>Voltaric</t>
   </si>
@@ -754,6 +754,12 @@
   </si>
   <si>
     <t>Add Charge Token</t>
+  </si>
+  <si>
+    <t>Add Grapple Marker</t>
+  </si>
+  <si>
+    <t>Remove Grapple Marker</t>
   </si>
 </sst>
 </file>
@@ -1009,10 +1015,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2632,7 +2638,7 @@
   <dimension ref="A1:W38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2666,8 +2672,8 @@
       <c r="A1" s="32"/>
       <c r="B1" s="32"/>
       <c r="C1" s="19"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -3134,22 +3140,28 @@
         <v>72</v>
       </c>
       <c r="T10" s="20"/>
-      <c r="V10" s="34"/>
-      <c r="W10" s="34"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="25" t="s">
+      <c r="A11" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="24" t="s">
         <v>73</v>
       </c>
+      <c r="C11" s="21" t="s">
+        <v>243</v>
+      </c>
       <c r="D11" s="20"/>
-      <c r="E11" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F11" s="25" t="s">
+      <c r="E11" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="24" t="s">
         <v>73</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>244</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="2" t="s">
@@ -3173,8 +3185,8 @@
         <v>73</v>
       </c>
       <c r="T11" s="20"/>
-      <c r="V11" s="34"/>
-      <c r="W11" s="34"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
@@ -3218,8 +3230,8 @@
         <v>74</v>
       </c>
       <c r="T12" s="20"/>
-      <c r="V12" s="34"/>
-      <c r="W12" s="34"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="33"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
@@ -3260,8 +3272,8 @@
         <v>75</v>
       </c>
       <c r="T13" s="20"/>
-      <c r="V13" s="34"/>
-      <c r="W13" s="34"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="33"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
@@ -3311,8 +3323,8 @@
         <v>76</v>
       </c>
       <c r="T14" s="20"/>
-      <c r="V14" s="34"/>
-      <c r="W14" s="34"/>
+      <c r="V14" s="33"/>
+      <c r="W14" s="33"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
@@ -3362,8 +3374,8 @@
         <v>77</v>
       </c>
       <c r="T15" s="20"/>
-      <c r="V15" s="34"/>
-      <c r="W15" s="34"/>
+      <c r="V15" s="33"/>
+      <c r="W15" s="33"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
@@ -3404,8 +3416,8 @@
         <v>78</v>
       </c>
       <c r="T16" s="20"/>
-      <c r="V16" s="34"/>
-      <c r="W16" s="34"/>
+      <c r="V16" s="33"/>
+      <c r="W16" s="33"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
@@ -3452,8 +3464,8 @@
         <v>79</v>
       </c>
       <c r="T17" s="20"/>
-      <c r="V17" s="34"/>
-      <c r="W17" s="34"/>
+      <c r="V17" s="33"/>
+      <c r="W17" s="33"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
@@ -3494,8 +3506,8 @@
         <v>80</v>
       </c>
       <c r="T18" s="20"/>
-      <c r="V18" s="34"/>
-      <c r="W18" s="34"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
@@ -3545,8 +3557,8 @@
         <v>81</v>
       </c>
       <c r="T19" s="20"/>
-      <c r="V19" s="34"/>
-      <c r="W19" s="34"/>
+      <c r="V19" s="33"/>
+      <c r="W19" s="33"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
@@ -3599,8 +3611,8 @@
         <v>240</v>
       </c>
       <c r="T20" s="20"/>
-      <c r="V20" s="34"/>
-      <c r="W20" s="34"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="33"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
@@ -3647,8 +3659,8 @@
         <v>83</v>
       </c>
       <c r="T21" s="20"/>
-      <c r="V21" s="34"/>
-      <c r="W21" s="34"/>
+      <c r="V21" s="33"/>
+      <c r="W21" s="33"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -3686,8 +3698,8 @@
         <v>84</v>
       </c>
       <c r="T22" s="20"/>
-      <c r="V22" s="34"/>
-      <c r="W22" s="34"/>
+      <c r="V22" s="33"/>
+      <c r="W22" s="33"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
@@ -3734,8 +3746,8 @@
         <v>85</v>
       </c>
       <c r="T23" s="20"/>
-      <c r="V23" s="34"/>
-      <c r="W23" s="34"/>
+      <c r="V23" s="33"/>
+      <c r="W23" s="33"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
@@ -3788,8 +3800,8 @@
         <v>241</v>
       </c>
       <c r="T24" s="20"/>
-      <c r="V24" s="34"/>
-      <c r="W24" s="34"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="33"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -3827,8 +3839,8 @@
         <v>87</v>
       </c>
       <c r="T25" s="20"/>
-      <c r="V25" s="34"/>
-      <c r="W25" s="34"/>
+      <c r="V25" s="33"/>
+      <c r="W25" s="33"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -3866,8 +3878,8 @@
         <v>88</v>
       </c>
       <c r="T26" s="20"/>
-      <c r="V26" s="34"/>
-      <c r="W26" s="34"/>
+      <c r="V26" s="33"/>
+      <c r="W26" s="33"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
@@ -3911,8 +3923,8 @@
         <v>89</v>
       </c>
       <c r="T27" s="20"/>
-      <c r="V27" s="34"/>
-      <c r="W27" s="34"/>
+      <c r="V27" s="33"/>
+      <c r="W27" s="33"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
@@ -3947,8 +3959,8 @@
       <c r="L28" s="20"/>
       <c r="P28" s="20"/>
       <c r="T28" s="20"/>
-      <c r="V28" s="34"/>
-      <c r="W28" s="34"/>
+      <c r="V28" s="33"/>
+      <c r="W28" s="33"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
@@ -3961,11 +3973,11 @@
         <v>131</v>
       </c>
       <c r="D29" s="20"/>
-      <c r="E29" s="33" t="s">
+      <c r="E29" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
       <c r="H29" s="20"/>
       <c r="I29" s="23" t="s">
         <v>90</v>
@@ -3979,8 +3991,8 @@
       <c r="L29" s="20"/>
       <c r="P29" s="20"/>
       <c r="T29" s="20"/>
-      <c r="V29" s="34"/>
-      <c r="W29" s="34"/>
+      <c r="V29" s="33"/>
+      <c r="W29" s="33"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
@@ -4015,8 +4027,8 @@
       <c r="L30" s="20"/>
       <c r="P30" s="20"/>
       <c r="T30" s="20"/>
-      <c r="V30" s="34"/>
-      <c r="W30" s="34"/>
+      <c r="V30" s="33"/>
+      <c r="W30" s="33"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
@@ -4051,8 +4063,8 @@
       <c r="L31" s="20"/>
       <c r="P31" s="20"/>
       <c r="T31" s="20"/>
-      <c r="V31" s="34"/>
-      <c r="W31" s="34"/>
+      <c r="V31" s="33"/>
+      <c r="W31" s="33"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
@@ -4087,8 +4099,8 @@
       <c r="L32" s="20"/>
       <c r="P32" s="20"/>
       <c r="T32" s="20"/>
-      <c r="V32" s="34"/>
-      <c r="W32" s="34"/>
+      <c r="V32" s="33"/>
+      <c r="W32" s="33"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -4116,8 +4128,8 @@
       <c r="L33" s="20"/>
       <c r="P33" s="20"/>
       <c r="T33" s="20"/>
-      <c r="V33" s="34"/>
-      <c r="W33" s="34"/>
+      <c r="V33" s="33"/>
+      <c r="W33" s="33"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
@@ -4266,17 +4278,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="V33:W33"/>
-    <mergeCell ref="V25:W25"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="V23:W23"/>
-    <mergeCell ref="V24:W24"/>
-    <mergeCell ref="V30:W30"/>
-    <mergeCell ref="V31:W31"/>
-    <mergeCell ref="V32:W32"/>
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="V1:W1"/>
@@ -4293,6 +4294,17 @@
     <mergeCell ref="V20:W20"/>
     <mergeCell ref="V21:W21"/>
     <mergeCell ref="V22:W22"/>
+    <mergeCell ref="V23:W23"/>
+    <mergeCell ref="V24:W24"/>
+    <mergeCell ref="V30:W30"/>
+    <mergeCell ref="V31:W31"/>
+    <mergeCell ref="V32:W32"/>
+    <mergeCell ref="V33:W33"/>
+    <mergeCell ref="V25:W25"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="V29:W29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>